<commit_message>
New Appendix on using Digital Multimeters
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -913,7 +913,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="229">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1599,6 +1599,12 @@
   </si>
   <si>
     <t>16 The Electric Field and the Electric Potential IV</t>
+  </si>
+  <si>
+    <t>Using Digital Multimeters</t>
+  </si>
+  <si>
+    <t>New in fall 2019, by MT</t>
   </si>
 </sst>
 </file>
@@ -2823,11 +2829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE116"/>
+  <dimension ref="A1:AE117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4398,15 +4404,15 @@
         <v>0</v>
       </c>
       <c r="Y26" s="6">
-        <f t="shared" ref="Y26:Y34" si="2">SUMIF(V$2:V$79,"&gt;=" &amp; X26,F$2:F$79)</f>
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,F$2:F$80)</f>
         <v>340</v>
       </c>
       <c r="Z26" s="6">
-        <f t="shared" ref="Z26:Z34" si="3">SUMIF(V$2:V$79,"&gt;=" &amp; X26,E$2:E$79)</f>
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,E$2:E$80)</f>
         <v>17</v>
       </c>
       <c r="AA26" s="8">
-        <f t="shared" ref="AA26:AA34" si="4">($Z$17 + $Z$15*Y26+$Z$16*Z26)*(1+Z$18+Z$19)</f>
+        <f t="shared" ref="AA26:AA34" si="2">($Z$17 + $Z$15*Y26+$Z$16*Z26)*(1+Z$18+Z$19)</f>
         <v>32.630000000000003</v>
       </c>
       <c r="AB26" s="33"/>
@@ -4473,15 +4479,15 @@
         <v>0.5</v>
       </c>
       <c r="Y27" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,F$2:F$80)</f>
+        <v>284</v>
+      </c>
+      <c r="Z27" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,E$2:E$80)</f>
+        <v>14</v>
+      </c>
+      <c r="AA27" s="8">
         <f t="shared" si="2"/>
-        <v>284</v>
-      </c>
-      <c r="Z27" s="6">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="AA27" s="8">
-        <f t="shared" si="4"/>
         <v>27.820000000000004</v>
       </c>
       <c r="AB27" s="33"/>
@@ -4556,15 +4562,15 @@
         <v>1</v>
       </c>
       <c r="Y28" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,F$2:F$80)</f>
+        <v>252</v>
+      </c>
+      <c r="Z28" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,E$2:E$80)</f>
+        <v>14</v>
+      </c>
+      <c r="AA28" s="8">
         <f t="shared" si="2"/>
-        <v>252</v>
-      </c>
-      <c r="Z28" s="6">
-        <f t="shared" si="3"/>
-        <v>14</v>
-      </c>
-      <c r="AA28" s="8">
-        <f t="shared" si="4"/>
         <v>25.740000000000002</v>
       </c>
     </row>
@@ -4610,15 +4616,15 @@
         <v>1.5</v>
       </c>
       <c r="Y29" s="31">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,F$2:F$80)</f>
+        <v>186</v>
+      </c>
+      <c r="Z29" s="31">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,E$2:E$80)</f>
+        <v>9</v>
+      </c>
+      <c r="AA29" s="8">
         <f t="shared" si="2"/>
-        <v>186</v>
-      </c>
-      <c r="Z29" s="31">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="AA29" s="8">
-        <f t="shared" si="4"/>
         <v>19.5</v>
       </c>
       <c r="AB29" s="33"/>
@@ -4665,15 +4671,15 @@
         <v>2</v>
       </c>
       <c r="Y30" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,F$2:F$80)</f>
+        <v>172</v>
+      </c>
+      <c r="Z30" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,E$2:E$80)</f>
+        <v>9</v>
+      </c>
+      <c r="AA30" s="8">
         <f t="shared" si="2"/>
-        <v>172</v>
-      </c>
-      <c r="Z30" s="6">
-        <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="AA30" s="8">
-        <f t="shared" si="4"/>
         <v>18.59</v>
       </c>
     </row>
@@ -4733,15 +4739,15 @@
         <v>2.5</v>
       </c>
       <c r="Y31" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,F$2:F$80)</f>
+        <v>126</v>
+      </c>
+      <c r="Z31" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,E$2:E$80)</f>
+        <v>4</v>
+      </c>
+      <c r="AA31" s="8">
         <f t="shared" si="2"/>
-        <v>126</v>
-      </c>
-      <c r="Z31" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="AA31" s="8">
-        <f t="shared" si="4"/>
         <v>13.65</v>
       </c>
       <c r="AB31" s="33"/>
@@ -4820,15 +4826,15 @@
         <v>3</v>
       </c>
       <c r="Y32" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X32,F$2:F$80)</f>
+        <v>100</v>
+      </c>
+      <c r="Z32" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X32,E$2:E$80)</f>
+        <v>4</v>
+      </c>
+      <c r="AA32" s="8">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="Z32" s="6">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="AA32" s="8">
-        <f t="shared" si="4"/>
         <v>11.959999999999999</v>
       </c>
     </row>
@@ -4894,15 +4900,15 @@
         <v>3.5</v>
       </c>
       <c r="Y33" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X33,F$2:F$80)</f>
+        <v>40</v>
+      </c>
+      <c r="Z33" s="6">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X33,E$2:E$80)</f>
+        <v>0</v>
+      </c>
+      <c r="AA33" s="8">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="Z33" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA33" s="8">
-        <f t="shared" si="4"/>
         <v>6.5</v>
       </c>
       <c r="AB33"/>
@@ -4981,15 +4987,15 @@
         <v>4</v>
       </c>
       <c r="Y34" s="47">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X34,F$2:F$80)</f>
+        <v>34</v>
+      </c>
+      <c r="Z34" s="47">
+        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X34,E$2:E$80)</f>
+        <v>0</v>
+      </c>
+      <c r="AA34" s="9">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="Z34" s="47">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA34" s="9">
-        <f t="shared" si="4"/>
         <v>6.11</v>
       </c>
     </row>
@@ -7060,7 +7066,7 @@
       </c>
       <c r="U71" s="84"/>
       <c r="V71" s="75">
-        <f t="shared" ref="V71:V78" si="5">SUM(R71:U71)</f>
+        <f t="shared" ref="V71:V79" si="3">SUM(R71:U71)</f>
         <v>2</v>
       </c>
       <c r="X71" s="3"/>
@@ -7085,7 +7091,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="14">
-        <f t="shared" ref="F72:F78" si="6">CEILING(D72,X$22+1)</f>
+        <f t="shared" ref="F72:F79" si="4">CEILING(D72,X$22+1)</f>
         <v>2</v>
       </c>
       <c r="K72" s="22" t="s">
@@ -7111,165 +7117,172 @@
       </c>
       <c r="U72" s="85"/>
       <c r="V72" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="W72" s="33"/>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B73" s="23" t="s">
+    <row r="73" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="30"/>
+      <c r="B73" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="C73" s="31"/>
+      <c r="D73" s="14">
+        <v>1</v>
+      </c>
+      <c r="E73" s="14">
+        <v>1</v>
+      </c>
+      <c r="F73" s="14">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="L73" s="85"/>
+      <c r="M73" s="85"/>
+      <c r="N73" s="85"/>
+      <c r="O73" s="85"/>
+      <c r="P73" s="85"/>
+      <c r="Q73" s="85"/>
+      <c r="R73" s="85"/>
+      <c r="S73" s="85"/>
+      <c r="T73" s="85"/>
+      <c r="U73" s="85"/>
+      <c r="V73" s="75"/>
+      <c r="X73" s="3"/>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B74" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="D73" s="14">
+      <c r="D74" s="14">
         <v>4</v>
       </c>
-      <c r="E73" s="14">
+      <c r="E74" s="14">
         <v>3</v>
       </c>
-      <c r="F73" s="14">
-        <f t="shared" si="6"/>
+      <c r="F74" s="14">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="K73" s="22"/>
-      <c r="L73" s="2">
-        <v>1</v>
-      </c>
-      <c r="M73" s="20">
-        <v>1</v>
-      </c>
-      <c r="N73" s="34">
-        <v>1</v>
-      </c>
-      <c r="O73" s="81">
-        <v>1</v>
-      </c>
-      <c r="P73" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="83">
-        <v>1</v>
-      </c>
-      <c r="R73" s="83">
-        <v>1</v>
-      </c>
-      <c r="T73" s="83">
-        <v>1</v>
-      </c>
-      <c r="U73" s="83">
-        <v>1</v>
-      </c>
-      <c r="V73" s="75">
-        <f t="shared" si="5"/>
+      <c r="K74" s="22"/>
+      <c r="L74" s="2">
+        <v>1</v>
+      </c>
+      <c r="M74" s="20">
+        <v>1</v>
+      </c>
+      <c r="N74" s="34">
+        <v>1</v>
+      </c>
+      <c r="O74" s="81">
+        <v>1</v>
+      </c>
+      <c r="P74" s="83">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="83">
+        <v>1</v>
+      </c>
+      <c r="R74" s="83">
+        <v>1</v>
+      </c>
+      <c r="T74" s="83">
+        <v>1</v>
+      </c>
+      <c r="U74" s="83">
+        <v>1</v>
+      </c>
+      <c r="V74" s="75">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="W73" s="33"/>
-      <c r="Y73" s="33"/>
-      <c r="Z73" s="33"/>
-      <c r="AA73" s="33"/>
-    </row>
-    <row r="74" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="10"/>
-      <c r="B74" s="23" t="s">
+      <c r="W74" s="33"/>
+      <c r="Y74" s="33"/>
+      <c r="Z74" s="33"/>
+      <c r="AA74" s="33"/>
+    </row>
+    <row r="75" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="10"/>
+      <c r="B75" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="C74" s="23"/>
-      <c r="D74" s="14">
-        <v>1</v>
-      </c>
-      <c r="E74" s="14">
-        <v>0</v>
-      </c>
-      <c r="F74" s="14">
-        <f t="shared" si="6"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="14">
+        <v>1</v>
+      </c>
+      <c r="E75" s="14">
+        <v>0</v>
+      </c>
+      <c r="F75" s="14">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="22" t="s">
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="L74" s="2"/>
-      <c r="M74" s="20">
-        <v>1</v>
-      </c>
-      <c r="N74" s="34">
-        <v>1</v>
-      </c>
-      <c r="O74" s="81">
-        <v>1</v>
-      </c>
-      <c r="P74" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="83">
-        <v>1</v>
-      </c>
-      <c r="R74" s="83">
-        <v>1</v>
-      </c>
-      <c r="S74" s="83"/>
-      <c r="T74" s="83">
-        <v>1</v>
-      </c>
-      <c r="U74" s="83"/>
-      <c r="V74" s="75">
-        <f t="shared" si="5"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="20">
+        <v>1</v>
+      </c>
+      <c r="N75" s="34">
+        <v>1</v>
+      </c>
+      <c r="O75" s="81">
+        <v>1</v>
+      </c>
+      <c r="P75" s="83">
+        <v>1</v>
+      </c>
+      <c r="Q75" s="83">
+        <v>1</v>
+      </c>
+      <c r="R75" s="83">
+        <v>1</v>
+      </c>
+      <c r="S75" s="83"/>
+      <c r="T75" s="83">
+        <v>1</v>
+      </c>
+      <c r="U75" s="83"/>
+      <c r="V75" s="75">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="W74" s="15"/>
-      <c r="X74" s="3"/>
-      <c r="Y74"/>
-      <c r="Z74" s="33"/>
-      <c r="AA74"/>
-      <c r="AB74" s="33"/>
-      <c r="AC74" s="33"/>
-      <c r="AD74" s="33"/>
-      <c r="AE74" s="33"/>
-    </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B75" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D75" s="14">
-        <v>3</v>
-      </c>
-      <c r="E75" s="14">
-        <v>1</v>
-      </c>
-      <c r="F75" s="14">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="K75" s="22"/>
-      <c r="N75" s="34"/>
-      <c r="O75" s="33"/>
-      <c r="P75" s="33"/>
-      <c r="Q75" s="33"/>
-      <c r="R75" s="33"/>
-      <c r="S75" s="33"/>
-      <c r="T75" s="33"/>
-      <c r="U75" s="33"/>
-      <c r="V75" s="75">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
       <c r="W75" s="15"/>
+      <c r="X75" s="3"/>
+      <c r="Y75"/>
+      <c r="Z75" s="33"/>
+      <c r="AA75"/>
+      <c r="AB75" s="33"/>
+      <c r="AC75" s="33"/>
+      <c r="AD75" s="33"/>
+      <c r="AE75" s="33"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B76" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D76" s="14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E76" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F76" s="14">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="K76" s="22"/>
       <c r="N76" s="34"/>
@@ -7281,33 +7294,27 @@
       <c r="T76" s="33"/>
       <c r="U76" s="33"/>
       <c r="V76" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W76" s="15"/>
-      <c r="AB76" s="6"/>
-      <c r="AC76" s="6"/>
-      <c r="AD76" s="6"/>
-      <c r="AE76" s="6"/>
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B77" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D77" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E77" s="14">
         <v>0</v>
       </c>
       <c r="F77" s="14">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="K77" s="22"/>
-      <c r="L77" s="83"/>
-      <c r="M77" s="85"/>
-      <c r="N77" s="83"/>
+      <c r="N77" s="34"/>
       <c r="O77" s="33"/>
       <c r="P77" s="33"/>
       <c r="Q77" s="33"/>
@@ -7316,145 +7323,143 @@
       <c r="T77" s="33"/>
       <c r="U77" s="33"/>
       <c r="V77" s="75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W77" s="15"/>
-    </row>
-    <row r="78" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="10"/>
-      <c r="B78" s="24" t="s">
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6"/>
+      <c r="AD77" s="6"/>
+      <c r="AE77" s="6"/>
+    </row>
+    <row r="78" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B78" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="14">
+        <v>4</v>
+      </c>
+      <c r="E78" s="14">
+        <v>0</v>
+      </c>
+      <c r="F78" s="14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K78" s="22"/>
+      <c r="L78" s="83"/>
+      <c r="M78" s="85"/>
+      <c r="N78" s="83"/>
+      <c r="O78" s="33"/>
+      <c r="P78" s="33"/>
+      <c r="Q78" s="33"/>
+      <c r="R78" s="33"/>
+      <c r="S78" s="33"/>
+      <c r="T78" s="33"/>
+      <c r="U78" s="33"/>
+      <c r="V78" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W78" s="15"/>
+    </row>
+    <row r="79" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="10"/>
+      <c r="B79" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="C78" s="24"/>
-      <c r="D78" s="27">
-        <v>1</v>
-      </c>
-      <c r="E78" s="27">
-        <v>0</v>
-      </c>
-      <c r="F78" s="27">
-        <f t="shared" si="6"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="27">
+        <v>1</v>
+      </c>
+      <c r="E79" s="27">
+        <v>0</v>
+      </c>
+      <c r="F79" s="27">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G78" s="27"/>
-      <c r="H78" s="27"/>
-      <c r="I78" s="27"/>
-      <c r="J78" s="27"/>
-      <c r="K78" s="29" t="s">
+      <c r="G79" s="27"/>
+      <c r="H79" s="27"/>
+      <c r="I79" s="27"/>
+      <c r="J79" s="27"/>
+      <c r="K79" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="L78" s="28"/>
-      <c r="M78" s="28">
-        <v>1</v>
-      </c>
-      <c r="N78" s="37"/>
-      <c r="O78" s="37">
-        <v>1</v>
-      </c>
-      <c r="P78" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q78" s="86">
-        <v>1</v>
-      </c>
-      <c r="R78" s="86"/>
-      <c r="S78" s="86">
-        <v>1</v>
-      </c>
-      <c r="T78" s="86">
-        <v>1</v>
-      </c>
-      <c r="U78" s="86"/>
-      <c r="V78" s="89">
-        <f t="shared" si="5"/>
+      <c r="L79" s="28"/>
+      <c r="M79" s="28">
+        <v>1</v>
+      </c>
+      <c r="N79" s="37"/>
+      <c r="O79" s="37">
+        <v>1</v>
+      </c>
+      <c r="P79" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q79" s="86">
+        <v>1</v>
+      </c>
+      <c r="R79" s="86"/>
+      <c r="S79" s="86">
+        <v>1</v>
+      </c>
+      <c r="T79" s="86">
+        <v>1</v>
+      </c>
+      <c r="U79" s="86"/>
+      <c r="V79" s="89">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="W78" s="15"/>
-      <c r="X78" s="3"/>
-      <c r="Y78"/>
-      <c r="Z78"/>
-      <c r="AA78"/>
-      <c r="AB78" s="6"/>
-      <c r="AC78" s="6"/>
-      <c r="AD78" s="6"/>
-      <c r="AE78" s="6"/>
-    </row>
-    <row r="79" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="11"/>
-    </row>
-    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="K80" s="64" t="s">
+      <c r="W79" s="15"/>
+      <c r="X79" s="3"/>
+      <c r="Y79"/>
+      <c r="Z79"/>
+      <c r="AA79"/>
+      <c r="AB79" s="6"/>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+      <c r="AE79" s="6"/>
+    </row>
+    <row r="80" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="11"/>
+    </row>
+    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="K81" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="L80" s="65">
-        <f t="array" ref="L80">SUM($F2:$F78*(L2:L78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="L81" s="65">
+        <f t="array" ref="L81">SUM($F2:$F79*(L2:L79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>104</v>
       </c>
-      <c r="M80" s="65">
-        <f t="array" ref="M80">SUM($F2:$F78*(M2:M78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="M81" s="65">
+        <f t="array" ref="M81">SUM($F2:$F79*(M2:M79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>136</v>
       </c>
-      <c r="N80" s="65">
-        <f t="array" ref="N80">SUM($F2:$F78*(N2:N78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="N81" s="65">
+        <f t="array" ref="N81">SUM($F2:$F79*(N2:N79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>144</v>
       </c>
-      <c r="O80" s="65">
-        <f t="array" ref="O80">SUM($F2:$F78*(O2:O78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="O81" s="65">
+        <f t="array" ref="O81">SUM($F2:$F79*(O2:O79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>140</v>
       </c>
-      <c r="P80" s="65">
-        <f t="array" ref="P80">SUM($F2:$F78*(P2:P78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="P81" s="65">
+        <f t="array" ref="P81">SUM($F2:$F79*(P2:P79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>144</v>
       </c>
-      <c r="Q80" s="66">
-        <f t="array" ref="Q80">SUM($F2:$F78*(Q2:Q78&gt;=0.9)*($V2:$V78&gt;=$X$12))</f>
+      <c r="Q81" s="66">
+        <f t="array" ref="Q81">SUM($F2:$F79*(Q2:Q79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
         <v>134</v>
-      </c>
-      <c r="R80" s="68"/>
-      <c r="S80" s="68"/>
-      <c r="T80" s="68"/>
-      <c r="U80" s="68"/>
-      <c r="Y80" s="33"/>
-      <c r="Z80" s="33"/>
-      <c r="AA80" s="33"/>
-      <c r="AB80" s="6"/>
-      <c r="AC80" s="6"/>
-      <c r="AD80" s="6"/>
-      <c r="AE80" s="6"/>
-    </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="K81" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="L81" s="68">
-        <f t="array" ref="L81">SUM($F2:$F78*L2:L78*($V2:$V78&gt;=$X$12))</f>
-        <v>106</v>
-      </c>
-      <c r="M81" s="68">
-        <f t="array" ref="M81">SUM($F2:$F78*M2:M78*($V2:$V78&gt;=$X$12))</f>
-        <v>143.4</v>
-      </c>
-      <c r="N81" s="68">
-        <f t="array" ref="N81">SUM($F2:$F78*N2:N78*($V2:$V78&gt;=$X$12))</f>
-        <v>145</v>
-      </c>
-      <c r="O81" s="68">
-        <f t="array" ref="O81">SUM($F2:$F78*O2:O78*($V2:$V78&gt;=$X$12))</f>
-        <v>151.6</v>
-      </c>
-      <c r="P81" s="68">
-        <f t="array" ref="P81">SUM($F2:$F78*P2:P78*($V2:$V78&gt;=$X$12))</f>
-        <v>149.80000000000001</v>
-      </c>
-      <c r="Q81" s="69">
-        <f t="array" ref="Q81">SUM($F2:$F78*Q2:Q78*($V2:$V78&gt;=$X$12))</f>
-        <v>147</v>
       </c>
       <c r="R81" s="68"/>
       <c r="S81" s="68"/>
       <c r="T81" s="68"/>
       <c r="U81" s="68"/>
+      <c r="Y81" s="33"/>
+      <c r="Z81" s="33"/>
+      <c r="AA81" s="33"/>
       <c r="AB81" s="6"/>
       <c r="AC81" s="6"/>
       <c r="AD81" s="6"/>
@@ -7462,64 +7467,68 @@
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K82" s="67" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L82" s="68">
-        <f t="array" ref="L82">SUM($F$2:$F$78*(L$2:L$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>108</v>
+        <f t="array" ref="L82">SUM($F2:$F79*L2:L79*($V2:$V79&gt;=$X$12))</f>
+        <v>106</v>
       </c>
       <c r="M82" s="68">
-        <f t="array" ref="M82">SUM($F$2:$F$78*(M$2:M$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>156</v>
+        <f t="array" ref="M82">SUM($F2:$F79*M2:M79*($V2:$V79&gt;=$X$12))</f>
+        <v>143.4</v>
       </c>
       <c r="N82" s="68">
-        <f t="array" ref="N82">SUM($F$2:$F$78*(N$2:N$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>146</v>
+        <f t="array" ref="N82">SUM($F2:$F79*N2:N79*($V2:$V79&gt;=$X$12))</f>
+        <v>145</v>
       </c>
       <c r="O82" s="68">
-        <f t="array" ref="O82">SUM($F$2:$F$78*(O$2:O$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>156</v>
+        <f t="array" ref="O82">SUM($F2:$F79*O2:O79*($V2:$V79&gt;=$X$12))</f>
+        <v>151.6</v>
       </c>
       <c r="P82" s="68">
-        <f t="array" ref="P82">SUM($F$2:$F$78*(P$2:P$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>154</v>
+        <f t="array" ref="P82">SUM($F2:$F79*P2:P79*($V2:$V79&gt;=$X$12))</f>
+        <v>149.80000000000001</v>
       </c>
       <c r="Q82" s="69">
-        <f t="array" ref="Q82">SUM($F$2:$F$78*(Q$2:Q$78&gt;=0.1)*($V$2:$V$78&gt;=$X$12))</f>
-        <v>162</v>
+        <f t="array" ref="Q82">SUM($F2:$F79*Q2:Q79*($V2:$V79&gt;=$X$12))</f>
+        <v>147</v>
       </c>
       <c r="R82" s="68"/>
       <c r="S82" s="68"/>
       <c r="T82" s="68"/>
       <c r="U82" s="68"/>
+      <c r="AB82" s="6"/>
+      <c r="AC82" s="6"/>
+      <c r="AD82" s="6"/>
+      <c r="AE82" s="6"/>
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K83" s="67" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L83" s="68">
-        <f t="shared" ref="L83:Q83" si="7">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
-        <v>186</v>
+        <f t="array" ref="L83">SUM($F$2:$F$79*(L$2:L$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>108</v>
       </c>
       <c r="M83" s="68">
-        <f t="shared" si="7"/>
-        <v>186</v>
+        <f t="array" ref="M83">SUM($F$2:$F$79*(M$2:M$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>156</v>
       </c>
       <c r="N83" s="68">
-        <f t="shared" si="7"/>
-        <v>186</v>
+        <f t="array" ref="N83">SUM($F$2:$F$79*(N$2:N$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>146</v>
       </c>
       <c r="O83" s="68">
-        <f t="shared" si="7"/>
-        <v>186</v>
+        <f t="array" ref="O83">SUM($F$2:$F$79*(O$2:O$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>156</v>
       </c>
       <c r="P83" s="68">
-        <f t="shared" si="7"/>
-        <v>186</v>
+        <f t="array" ref="P83">SUM($F$2:$F$79*(P$2:P$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>154</v>
       </c>
       <c r="Q83" s="69">
-        <f t="shared" si="7"/>
-        <v>186</v>
+        <f t="array" ref="Q83">SUM($F$2:$F$79*(Q$2:Q$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+        <v>162</v>
       </c>
       <c r="R83" s="68"/>
       <c r="S83" s="68"/>
@@ -7528,136 +7537,169 @@
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K84" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="L84" s="68">
+        <f t="shared" ref="L84:Q84" si="5">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
+        <v>186</v>
+      </c>
+      <c r="M84" s="68">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="N84" s="68">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="O84" s="68">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="P84" s="68">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="Q84" s="69">
+        <f t="shared" si="5"/>
+        <v>186</v>
+      </c>
+      <c r="R84" s="68"/>
+      <c r="S84" s="68"/>
+      <c r="T84" s="68"/>
+      <c r="U84" s="68"/>
+    </row>
+    <row r="85" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="K85" s="67" t="s">
         <v>169</v>
       </c>
-      <c r="L84" s="70">
-        <f t="shared" ref="L84:N84" si="8">L81/L83</f>
+      <c r="L85" s="70">
+        <f t="shared" ref="L85:N85" si="6">L82/L84</f>
         <v>0.56989247311827962</v>
       </c>
-      <c r="M84" s="70">
-        <f t="shared" si="8"/>
+      <c r="M85" s="70">
+        <f t="shared" si="6"/>
         <v>0.7709677419354839</v>
       </c>
-      <c r="N84" s="70">
-        <f t="shared" si="8"/>
+      <c r="N85" s="70">
+        <f t="shared" si="6"/>
         <v>0.77956989247311825</v>
       </c>
-      <c r="O84" s="70">
-        <f t="shared" ref="O84:P84" si="9">O81/O83</f>
+      <c r="O85" s="70">
+        <f t="shared" ref="O85:P85" si="7">O82/O84</f>
         <v>0.81505376344086022</v>
       </c>
-      <c r="P84" s="70">
-        <f t="shared" si="9"/>
+      <c r="P85" s="70">
+        <f t="shared" si="7"/>
         <v>0.80537634408602155</v>
       </c>
-      <c r="Q84" s="71">
-        <f t="shared" ref="Q84" si="10">Q81/Q83</f>
+      <c r="Q85" s="71">
+        <f t="shared" ref="Q85" si="8">Q82/Q84</f>
         <v>0.79032258064516125</v>
       </c>
-      <c r="R84" s="70"/>
-      <c r="S84" s="70"/>
-      <c r="T84" s="70"/>
-      <c r="U84" s="70"/>
-    </row>
-    <row r="85" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D85" s="33"/>
-      <c r="K85" s="72" t="s">
+      <c r="R85" s="70"/>
+      <c r="S85" s="70"/>
+      <c r="T85" s="70"/>
+      <c r="U85" s="70"/>
+    </row>
+    <row r="86" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D86" s="33"/>
+      <c r="K86" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="L85" s="73">
-        <f t="array" ref="L85">SUM($F2:$F78*L2:L78*($V2:$V78&lt;$X$12))</f>
+      <c r="L86" s="73">
+        <f t="array" ref="L86">SUM($F2:$F79*L2:L79*($V2:$V79&lt;$X$12))</f>
         <v>10</v>
       </c>
-      <c r="M85" s="73">
-        <f t="array" ref="M85">SUM($F2:$F78*M2:M78*($V2:$V78&lt;$X$12))</f>
+      <c r="M86" s="73">
+        <f t="array" ref="M86">SUM($F2:$F79*M2:M79*($V2:$V79&lt;$X$12))</f>
         <v>31.6</v>
       </c>
-      <c r="N85" s="73">
-        <f t="array" ref="N85">SUM($F2:$F78*N2:N78*($V2:$V78&lt;$X$12))</f>
+      <c r="N86" s="73">
+        <f t="array" ref="N86">SUM($F2:$F79*N2:N79*($V2:$V79&lt;$X$12))</f>
         <v>32</v>
       </c>
-      <c r="O85" s="73">
-        <f t="array" ref="O85">SUM($F2:$F78*O2:O78*($V2:$V78&lt;$X$12))</f>
+      <c r="O86" s="73">
+        <f t="array" ref="O86">SUM($F2:$F79*O2:O79*($V2:$V79&lt;$X$12))</f>
         <v>17.8</v>
       </c>
-      <c r="P85" s="73">
-        <f t="array" ref="P85">SUM($F2:$F78*P2:P78*($V2:$V78&lt;$X$12))</f>
+      <c r="P86" s="73">
+        <f t="array" ref="P86">SUM($F2:$F79*P2:P79*($V2:$V79&lt;$X$12))</f>
         <v>19</v>
       </c>
-      <c r="Q85" s="74">
-        <f t="array" ref="Q85">SUM($F2:$F78*Q2:Q78*($V2:$V78&lt;$X$12))</f>
+      <c r="Q86" s="74">
+        <f t="array" ref="Q86">SUM($F2:$F79*Q2:Q79*($V2:$V79&lt;$X$12))</f>
         <v>19.3</v>
       </c>
-      <c r="R85" s="68"/>
-      <c r="S85" s="68"/>
-      <c r="T85" s="68"/>
-      <c r="U85" s="68"/>
-      <c r="AA85" s="33"/>
-    </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="D86" s="33"/>
+      <c r="R86" s="68"/>
+      <c r="S86" s="68"/>
+      <c r="T86" s="68"/>
+      <c r="U86" s="68"/>
+      <c r="AA86" s="33"/>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="D87" s="33"/>
     </row>
-    <row r="88" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="10"/>
-      <c r="B88" s="23"/>
-      <c r="C88" s="23"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="20"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="20"/>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="34"/>
-      <c r="Q88" s="83"/>
-      <c r="R88" s="83"/>
-      <c r="S88" s="83"/>
-      <c r="T88" s="83"/>
-      <c r="U88" s="83"/>
-      <c r="V88" s="3"/>
-      <c r="W88" s="3"/>
-      <c r="X88" s="3"/>
-      <c r="Y88"/>
-      <c r="Z88"/>
-      <c r="AA88"/>
-      <c r="AB88"/>
-      <c r="AC88"/>
-      <c r="AD88"/>
-      <c r="AE88"/>
-    </row>
-    <row r="94" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="AB94" s="6"/>
-      <c r="AC94" s="6"/>
-      <c r="AD94" s="6"/>
-      <c r="AE94" s="6"/>
-    </row>
-    <row r="98" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB98" s="6"/>
-      <c r="AC98" s="6"/>
-      <c r="AD98" s="6"/>
-      <c r="AE98" s="6"/>
-    </row>
-    <row r="103" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB103" s="6"/>
-      <c r="AC103" s="6"/>
-      <c r="AD103" s="6"/>
-      <c r="AE103" s="6"/>
-    </row>
-    <row r="116" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB116" s="33"/>
-      <c r="AC116" s="33"/>
-      <c r="AD116" s="33"/>
-      <c r="AE116" s="33"/>
+    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="D88" s="33"/>
+    </row>
+    <row r="89" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="10"/>
+      <c r="B89" s="23"/>
+      <c r="C89" s="23"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="20"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+      <c r="P89" s="34"/>
+      <c r="Q89" s="83"/>
+      <c r="R89" s="83"/>
+      <c r="S89" s="83"/>
+      <c r="T89" s="83"/>
+      <c r="U89" s="83"/>
+      <c r="V89" s="3"/>
+      <c r="W89" s="3"/>
+      <c r="X89" s="3"/>
+      <c r="Y89"/>
+      <c r="Z89"/>
+      <c r="AA89"/>
+      <c r="AB89"/>
+      <c r="AC89"/>
+      <c r="AD89"/>
+      <c r="AE89"/>
+    </row>
+    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AB95" s="6"/>
+      <c r="AC95" s="6"/>
+      <c r="AD95" s="6"/>
+      <c r="AE95" s="6"/>
+    </row>
+    <row r="99" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB99" s="6"/>
+      <c r="AC99" s="6"/>
+      <c r="AD99" s="6"/>
+      <c r="AE99" s="6"/>
+    </row>
+    <row r="104" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB104" s="6"/>
+      <c r="AC104" s="6"/>
+      <c r="AD104" s="6"/>
+      <c r="AE104" s="6"/>
+    </row>
+    <row r="117" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB117" s="33"/>
+      <c r="AC117" s="33"/>
+      <c r="AD117" s="33"/>
+      <c r="AE117" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:V78">
+  <conditionalFormatting sqref="B2:V79">
     <cfRule type="expression" dxfId="2" priority="40" stopIfTrue="1">
       <formula>$V2&gt;=(0.5+$X$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated spreadsheet for spring 2020
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -15,7 +15,7 @@
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -711,7 +711,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M46" authorId="0" shapeId="0">
+    <comment ref="M47" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M52" authorId="0" shapeId="0">
+    <comment ref="M54" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -761,7 +761,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M53" authorId="0" shapeId="0">
+    <comment ref="M55" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -786,7 +786,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M55" authorId="0" shapeId="0">
+    <comment ref="M57" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -810,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M58" authorId="0" shapeId="0">
+    <comment ref="M60" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -835,7 +835,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M61" authorId="0" shapeId="0">
+    <comment ref="M63" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -859,7 +859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M64" authorId="0" shapeId="0">
+    <comment ref="M66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -884,7 +884,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M71" authorId="0" shapeId="0">
+    <comment ref="M73" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -913,7 +913,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="232">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1251,9 +1251,6 @@
     <t>by MT 2015</t>
   </si>
   <si>
-    <t>Interference of Light from Multiple Slits</t>
-  </si>
-  <si>
     <t>Music to Our Ears: Standing Waves in Strings</t>
   </si>
   <si>
@@ -1605,6 +1602,18 @@
   </si>
   <si>
     <t>New in fall 2019, by MT</t>
+  </si>
+  <si>
+    <t>Interference of Light from Two or More Slits</t>
+  </si>
+  <si>
+    <t>The Interference of Light</t>
+  </si>
+  <si>
+    <t>Diffraction of Light</t>
+  </si>
+  <si>
+    <t>by Jerry, 2019, from older version</t>
   </si>
 </sst>
 </file>
@@ -2829,11 +2838,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE117"/>
+  <dimension ref="A1:AE119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,7 +2873,7 @@
         <v>107</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="50" t="s">
         <v>85</v>
@@ -2873,19 +2882,19 @@
         <v>86</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G1" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>181</v>
-      </c>
-      <c r="J1" s="50" t="s">
-        <v>182</v>
       </c>
       <c r="K1" s="51" t="s">
         <v>108</v>
@@ -2894,34 +2903,34 @@
         <v>109</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N1" s="49" t="s">
         <v>100</v>
       </c>
       <c r="O1" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P1" s="49" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q1" s="49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="R1" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="S1" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="T1" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="U1" s="49" t="s">
         <v>220</v>
       </c>
-      <c r="U1" s="49" t="s">
+      <c r="V1" s="52" t="s">
         <v>221</v>
-      </c>
-      <c r="V1" s="52" t="s">
-        <v>222</v>
       </c>
       <c r="W1" s="32"/>
       <c r="X1" s="33"/>
@@ -3009,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="61">
-        <f t="shared" ref="F3:F71" si="0">CEILING(D3,X$22+1)</f>
+        <f t="shared" ref="F3:F73" si="0">CEILING(D3,X$22+1)</f>
         <v>2</v>
       </c>
       <c r="G3" s="61"/>
@@ -3044,7 +3053,7 @@
       </c>
       <c r="U3" s="88"/>
       <c r="V3" s="89">
-        <f t="shared" ref="V3:V70" si="1">SUM(R3:U3)</f>
+        <f t="shared" ref="V3:V72" si="1">SUM(R3:U3)</f>
         <v>2</v>
       </c>
       <c r="W3" s="33"/>
@@ -3062,10 +3071,10 @@
         <v>73</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D4" s="14">
         <v>5</v>
@@ -3136,10 +3145,10 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D5" s="14">
         <v>2</v>
@@ -3208,10 +3217,10 @@
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D6" s="14">
         <v>2</v>
@@ -3269,10 +3278,10 @@
     <row r="7" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48"/>
       <c r="B7" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="27">
         <v>1</v>
@@ -3289,7 +3298,7 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L7" s="37"/>
       <c r="M7" s="37">
@@ -3319,10 +3328,10 @@
         <v>74</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D8" s="14">
         <v>4</v>
@@ -3341,7 +3350,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L8" s="34"/>
       <c r="M8" s="36">
@@ -3384,10 +3393,10 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" s="14">
         <v>2</v>
@@ -3448,10 +3457,10 @@
     </row>
     <row r="10" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D10" s="14">
         <v>5</v>
@@ -3503,10 +3512,10 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" s="14">
         <v>2</v>
@@ -3569,10 +3578,10 @@
     </row>
     <row r="12" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D12" s="14">
         <v>4</v>
@@ -3614,10 +3623,10 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D13" s="14">
         <v>3</v>
@@ -3657,10 +3666,10 @@
     </row>
     <row r="14" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" s="14">
         <v>3</v>
@@ -3695,10 +3704,10 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D15" s="14">
         <v>3</v>
@@ -3736,10 +3745,10 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D16" s="14">
         <v>9</v>
@@ -3752,7 +3761,7 @@
         <v>10</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L16" s="34"/>
       <c r="M16" s="36">
@@ -3799,10 +3808,10 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D17" s="14">
         <v>3</v>
@@ -3877,10 +3886,10 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D18" s="14">
         <v>5</v>
@@ -3893,7 +3902,7 @@
         <v>6</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L18" s="34"/>
       <c r="M18" s="36">
@@ -3943,10 +3952,10 @@
     </row>
     <row r="19" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D19" s="14">
         <v>4</v>
@@ -3959,7 +3968,7 @@
         <v>4</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L19" s="34"/>
       <c r="M19" s="36">
@@ -4006,10 +4015,10 @@
     </row>
     <row r="20" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D20" s="14">
         <v>5</v>
@@ -4070,10 +4079,10 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D21" s="14">
         <v>3</v>
@@ -4100,7 +4109,7 @@
       </c>
       <c r="W21" s="33"/>
       <c r="X21" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y21" s="43"/>
       <c r="Z21" s="33"/>
@@ -4112,10 +4121,10 @@
     </row>
     <row r="22" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D22" s="14">
         <v>4</v>
@@ -4159,10 +4168,10 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D23" s="14">
         <v>2</v>
@@ -4218,10 +4227,10 @@
         <v>75</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D24" s="13">
         <v>10</v>
@@ -4284,10 +4293,10 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D25" s="14">
         <v>8</v>
@@ -4347,16 +4356,16 @@
       </c>
       <c r="W25" s="33"/>
       <c r="X25" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y25" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="Y25" s="4" t="s">
+      <c r="Z25" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="Z25" s="4" t="s">
+      <c r="AA25" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="AA25" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="AB25" s="33"/>
       <c r="AC25" s="33"/>
@@ -4365,10 +4374,10 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26" s="14">
         <v>3</v>
@@ -4404,16 +4413,16 @@
         <v>0</v>
       </c>
       <c r="Y26" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,F$2:F$80)</f>
-        <v>340</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X26,F$2:F$82)</f>
+        <v>354</v>
       </c>
       <c r="Z26" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X26,E$2:E$80)</f>
-        <v>17</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X26,E$2:E$82)</f>
+        <v>24</v>
       </c>
       <c r="AA26" s="8">
         <f t="shared" ref="AA26:AA34" si="2">($Z$17 + $Z$15*Y26+$Z$16*Z26)*(1+Z$18+Z$19)</f>
-        <v>32.630000000000003</v>
+        <v>36.269999999999996</v>
       </c>
       <c r="AB26" s="33"/>
       <c r="AC26" s="33"/>
@@ -4422,10 +4431,10 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D27" s="14">
         <v>3</v>
@@ -4479,16 +4488,16 @@
         <v>0.5</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,F$2:F$80)</f>
-        <v>284</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X27,F$2:F$82)</f>
+        <v>286</v>
       </c>
       <c r="Z27" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X27,E$2:E$80)</f>
-        <v>14</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X27,E$2:E$82)</f>
+        <v>15</v>
       </c>
       <c r="AA27" s="8">
         <f t="shared" si="2"/>
-        <v>27.820000000000004</v>
+        <v>28.340000000000003</v>
       </c>
       <c r="AB27" s="33"/>
       <c r="AC27" s="33"/>
@@ -4498,10 +4507,10 @@
     <row r="28" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D28" s="14">
         <v>3</v>
@@ -4562,24 +4571,24 @@
         <v>1</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,F$2:F$80)</f>
-        <v>252</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X28,F$2:F$82)</f>
+        <v>254</v>
       </c>
       <c r="Z28" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X28,E$2:E$80)</f>
-        <v>14</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X28,E$2:E$82)</f>
+        <v>15</v>
       </c>
       <c r="AA28" s="8">
         <f t="shared" si="2"/>
-        <v>25.740000000000002</v>
+        <v>26.260000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D29" s="14">
         <v>5</v>
@@ -4595,7 +4604,7 @@
         <v>37</v>
       </c>
       <c r="K29" s="57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N29" s="34"/>
       <c r="O29" s="34">
@@ -4616,16 +4625,16 @@
         <v>1.5</v>
       </c>
       <c r="Y29" s="31">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,F$2:F$80)</f>
-        <v>186</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X29,F$2:F$82)</f>
+        <v>188</v>
       </c>
       <c r="Z29" s="31">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X29,E$2:E$80)</f>
-        <v>9</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X29,E$2:E$82)</f>
+        <v>10</v>
       </c>
       <c r="AA29" s="8">
         <f t="shared" si="2"/>
-        <v>19.5</v>
+        <v>20.02</v>
       </c>
       <c r="AB29" s="33"/>
       <c r="AC29" s="33"/>
@@ -4634,10 +4643,10 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D30" s="14">
         <v>5</v>
@@ -4650,7 +4659,7 @@
         <v>6</v>
       </c>
       <c r="K30" s="57" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N30" s="34"/>
       <c r="O30" s="34">
@@ -4671,16 +4680,16 @@
         <v>2</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,F$2:F$80)</f>
-        <v>172</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X30,F$2:F$82)</f>
+        <v>174</v>
       </c>
       <c r="Z30" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X30,E$2:E$80)</f>
-        <v>9</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X30,E$2:E$82)</f>
+        <v>10</v>
       </c>
       <c r="AA30" s="8">
         <f t="shared" si="2"/>
-        <v>18.59</v>
+        <v>19.110000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
@@ -4688,10 +4697,10 @@
         <v>77</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D31" s="13">
         <v>3</v>
@@ -4712,7 +4721,7 @@
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
@@ -4739,16 +4748,16 @@
         <v>2.5</v>
       </c>
       <c r="Y31" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,F$2:F$80)</f>
-        <v>126</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X31,F$2:F$82)</f>
+        <v>128</v>
       </c>
       <c r="Z31" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X31,E$2:E$80)</f>
-        <v>4</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X31,E$2:E$82)</f>
+        <v>5</v>
       </c>
       <c r="AA31" s="8">
         <f t="shared" si="2"/>
-        <v>13.65</v>
+        <v>14.170000000000002</v>
       </c>
       <c r="AB31" s="33"/>
       <c r="AC31" s="33"/>
@@ -4757,10 +4766,10 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B32" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D32" s="14">
         <v>2</v>
@@ -4785,7 +4794,7 @@
         <v>15</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L32" s="2">
         <v>1</v>
@@ -4826,25 +4835,25 @@
         <v>3</v>
       </c>
       <c r="Y32" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X32,F$2:F$80)</f>
-        <v>100</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X32,F$2:F$82)</f>
+        <v>102</v>
       </c>
       <c r="Z32" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X32,E$2:E$80)</f>
-        <v>4</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X32,E$2:E$82)</f>
+        <v>5</v>
       </c>
       <c r="AA32" s="8">
         <f t="shared" si="2"/>
-        <v>11.959999999999999</v>
+        <v>12.480000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D33" s="14">
         <v>1</v>
@@ -4863,7 +4872,7 @@
         <v>16</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L33" s="34"/>
       <c r="M33" s="36">
@@ -4900,16 +4909,16 @@
         <v>3.5</v>
       </c>
       <c r="Y33" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X33,F$2:F$80)</f>
-        <v>40</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X33,F$2:F$82)</f>
+        <v>42</v>
       </c>
       <c r="Z33" s="6">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X33,E$2:E$80)</f>
-        <v>0</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X33,E$2:E$82)</f>
+        <v>1</v>
       </c>
       <c r="AA33" s="8">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>7.02</v>
       </c>
       <c r="AB33"/>
       <c r="AC33"/>
@@ -4918,10 +4927,10 @@
     </row>
     <row r="34" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D34" s="14">
         <v>3</v>
@@ -4946,7 +4955,7 @@
         <v>16</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L34" s="2">
         <v>1</v>
@@ -4987,25 +4996,25 @@
         <v>4</v>
       </c>
       <c r="Y34" s="47">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X34,F$2:F$80)</f>
-        <v>34</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X34,F$2:F$82)</f>
+        <v>36</v>
       </c>
       <c r="Z34" s="47">
-        <f>SUMIF(V$2:V$80,"&gt;=" &amp; X34,E$2:E$80)</f>
-        <v>0</v>
+        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X34,E$2:E$82)</f>
+        <v>1</v>
       </c>
       <c r="AA34" s="9">
         <f t="shared" si="2"/>
-        <v>6.11</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="35" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D35" s="14">
         <v>3</v>
@@ -5064,7 +5073,7 @@
         <v>97</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D36" s="14">
         <v>2</v>
@@ -5124,7 +5133,7 @@
         <v>98</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D37" s="14">
         <v>4</v>
@@ -5140,7 +5149,7 @@
         <v>19</v>
       </c>
       <c r="K37" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M37" s="20">
         <v>1</v>
@@ -5177,7 +5186,7 @@
         <v>95</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D38" s="14">
         <v>3</v>
@@ -5193,7 +5202,7 @@
         <v>20</v>
       </c>
       <c r="K38" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M38" s="20">
         <v>1</v>
@@ -5228,10 +5237,10 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B39" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D39" s="14">
         <v>7</v>
@@ -5298,10 +5307,10 @@
         <v>78</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D40" s="13">
         <v>2</v>
@@ -5314,7 +5323,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H40" s="13">
         <v>23</v>
@@ -5326,7 +5335,7 @@
         <v>22</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L40" s="12">
         <v>1</v>
@@ -5367,10 +5376,10 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B41" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D41" s="14">
         <v>5</v>
@@ -5433,10 +5442,10 @@
     <row r="42" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D42" s="14">
         <v>4</v>
@@ -5453,7 +5462,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="20"/>
@@ -5483,10 +5492,10 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D43" s="14">
         <v>6</v>
@@ -5542,10 +5551,10 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D44" s="14">
         <v>5</v>
@@ -5558,7 +5567,7 @@
         <v>6</v>
       </c>
       <c r="G44" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H44" s="14">
         <v>26</v>
@@ -5570,7 +5579,7 @@
         <v>25</v>
       </c>
       <c r="K44" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M44" s="20">
         <v>1</v>
@@ -5605,23 +5614,23 @@
         <v>79</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>111</v>
+        <v>228</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D45" s="13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E45" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="13">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H45" s="13">
         <v>28</v>
@@ -5671,120 +5680,89 @@
       </c>
       <c r="W45" s="33"/>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B46" s="23" t="s">
-        <v>93</v>
+    <row r="46" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="31" t="s">
+        <v>229</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D46" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E46" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="H46" s="14">
-        <v>29</v>
-      </c>
-      <c r="I46" s="14">
-        <v>12</v>
-      </c>
-      <c r="J46" s="14">
-        <v>27</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
       <c r="K46" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="2">
-        <v>1</v>
-      </c>
-      <c r="M46" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="N46" s="34">
-        <v>1</v>
-      </c>
-      <c r="O46" s="34">
-        <v>0.8</v>
-      </c>
-      <c r="P46" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="83">
-        <v>1</v>
-      </c>
-      <c r="R46" s="83">
-        <v>1</v>
-      </c>
-      <c r="S46" s="83">
-        <v>1</v>
-      </c>
-      <c r="T46" s="83">
-        <v>1</v>
-      </c>
-      <c r="U46" s="83">
-        <v>1</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="L46" s="85"/>
+      <c r="M46" s="85"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
+      <c r="P46" s="85"/>
+      <c r="Q46" s="85"/>
+      <c r="R46" s="85"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="85"/>
+      <c r="U46" s="85"/>
       <c r="V46" s="75">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="W46" s="33"/>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6"/>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6"/>
-      <c r="AE46" s="6"/>
-    </row>
-    <row r="47" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="X46" s="3"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D47" s="14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E47" s="14">
         <v>0</v>
       </c>
       <c r="F47" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G47" s="14">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="G47" s="14" t="s">
+        <v>177</v>
       </c>
       <c r="H47" s="14">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I47" s="14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J47" s="14">
-        <v>28</v>
-      </c>
-      <c r="K47" s="22"/>
-      <c r="L47" s="83">
-        <v>1</v>
-      </c>
-      <c r="M47" s="85">
-        <v>0.4</v>
-      </c>
-      <c r="N47" s="83">
-        <v>1</v>
-      </c>
-      <c r="O47" s="83">
+        <v>27</v>
+      </c>
+      <c r="K47" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="L47" s="2">
+        <v>1</v>
+      </c>
+      <c r="M47" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="N47" s="34">
+        <v>1</v>
+      </c>
+      <c r="O47" s="34">
         <v>0.8</v>
       </c>
       <c r="P47" s="83">
@@ -5794,9 +5772,11 @@
         <v>1</v>
       </c>
       <c r="R47" s="83">
-        <v>0.5</v>
-      </c>
-      <c r="S47" s="83"/>
+        <v>1</v>
+      </c>
+      <c r="S47" s="83">
+        <v>1</v>
+      </c>
       <c r="T47" s="83">
         <v>1</v>
       </c>
@@ -5805,136 +5785,142 @@
       </c>
       <c r="V47" s="75">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="W47" s="33"/>
-      <c r="X47" s="15"/>
-      <c r="Z47"/>
-      <c r="AA47"/>
-      <c r="AB47"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
-      <c r="AE47"/>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6"/>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6"/>
+      <c r="AE47" s="6"/>
+    </row>
+    <row r="48" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
       <c r="B48" s="23" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D48" s="14">
+        <v>8</v>
+      </c>
+      <c r="E48" s="14">
         <v>4</v>
-      </c>
-      <c r="E48" s="14">
-        <v>0</v>
       </c>
       <c r="F48" s="14">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G48" s="14">
-        <v>43</v>
-      </c>
-      <c r="H48" s="14">
-        <v>30</v>
-      </c>
-      <c r="I48" s="14">
-        <v>13</v>
-      </c>
-      <c r="J48" s="14">
-        <v>28</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
       <c r="K48" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="N48" s="34"/>
-      <c r="O48" s="34"/>
-      <c r="P48" s="83">
-        <v>0.5</v>
-      </c>
-      <c r="Q48" s="83">
-        <v>0.7</v>
-      </c>
-      <c r="T48" s="83">
-        <v>0.75</v>
-      </c>
-      <c r="V48" s="89">
+        <v>231</v>
+      </c>
+      <c r="L48" s="83"/>
+      <c r="M48" s="85"/>
+      <c r="N48" s="83"/>
+      <c r="O48" s="83"/>
+      <c r="P48" s="83"/>
+      <c r="Q48" s="83"/>
+      <c r="R48" s="83"/>
+      <c r="S48" s="83"/>
+      <c r="T48" s="83"/>
+      <c r="U48" s="83"/>
+      <c r="V48" s="75">
         <f t="shared" si="1"/>
-        <v>0.75</v>
-      </c>
-      <c r="W48" s="33"/>
-      <c r="Z48" s="6"/>
-    </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="D49" s="13">
+        <v>0</v>
+      </c>
+      <c r="X48" s="3"/>
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6"/>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6"/>
+      <c r="AE48" s="6"/>
+    </row>
+    <row r="49" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D49" s="14">
         <v>2</v>
       </c>
-      <c r="E49" s="13">
-        <v>0</v>
-      </c>
-      <c r="F49" s="13">
+      <c r="E49" s="14">
+        <v>0</v>
+      </c>
+      <c r="F49" s="14">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G49" s="13">
-        <v>38</v>
-      </c>
-      <c r="H49" s="13">
-        <v>31</v>
-      </c>
-      <c r="I49" s="13">
-        <v>9</v>
-      </c>
-      <c r="J49" s="13"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="12">
-        <v>1</v>
-      </c>
-      <c r="M49" s="12"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="35"/>
-      <c r="P49" s="84">
-        <v>1</v>
-      </c>
-      <c r="Q49" s="84">
-        <v>0</v>
-      </c>
-      <c r="R49" s="84">
-        <v>1</v>
-      </c>
-      <c r="S49" s="84"/>
-      <c r="T49" s="84">
-        <v>0.75</v>
-      </c>
-      <c r="U49" s="84">
+      <c r="G49" s="14">
+        <v>43</v>
+      </c>
+      <c r="H49" s="14">
+        <v>30</v>
+      </c>
+      <c r="I49" s="14">
+        <v>13</v>
+      </c>
+      <c r="J49" s="14">
+        <v>28</v>
+      </c>
+      <c r="K49" s="22"/>
+      <c r="L49" s="83">
+        <v>1</v>
+      </c>
+      <c r="M49" s="85">
+        <v>0.4</v>
+      </c>
+      <c r="N49" s="83">
+        <v>1</v>
+      </c>
+      <c r="O49" s="83">
+        <v>0.8</v>
+      </c>
+      <c r="P49" s="83">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="83">
+        <v>1</v>
+      </c>
+      <c r="R49" s="83">
+        <v>0.5</v>
+      </c>
+      <c r="S49" s="83"/>
+      <c r="T49" s="83">
+        <v>1</v>
+      </c>
+      <c r="U49" s="83">
         <v>1</v>
       </c>
       <c r="V49" s="75">
         <f t="shared" si="1"/>
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="W49" s="33"/>
-    </row>
-    <row r="50" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
+      <c r="X49" s="15"/>
+      <c r="Z49"/>
+      <c r="AA49"/>
+      <c r="AB49"/>
+      <c r="AC49"/>
+      <c r="AD49"/>
+      <c r="AE49"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B50" s="23" t="s">
-        <v>133</v>
+        <v>215</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D50" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E50" s="14">
         <v>0</v>
@@ -5944,61 +5930,47 @@
         <v>4</v>
       </c>
       <c r="G50" s="14">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H50" s="14">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I50" s="14">
-        <v>10</v>
-      </c>
-      <c r="J50" s="14"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="2">
-        <v>1</v>
-      </c>
-      <c r="M50" s="20"/>
+        <v>13</v>
+      </c>
+      <c r="J50" s="14">
+        <v>28</v>
+      </c>
+      <c r="K50" s="22" t="s">
+        <v>214</v>
+      </c>
       <c r="N50" s="34"/>
       <c r="O50" s="34"/>
       <c r="P50" s="83">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q50" s="83">
-        <v>0</v>
-      </c>
-      <c r="R50" s="83">
-        <v>1</v>
-      </c>
-      <c r="S50" s="83"/>
+        <v>0.7</v>
+      </c>
       <c r="T50" s="83">
         <v>0.75</v>
       </c>
-      <c r="U50" s="83">
-        <v>1</v>
-      </c>
       <c r="V50" s="89">
         <f t="shared" si="1"/>
-        <v>2.75</v>
+        <v>0.75</v>
       </c>
       <c r="W50" s="33"/>
-      <c r="X50" s="3"/>
-      <c r="Y50"/>
-      <c r="Z50"/>
-      <c r="AA50"/>
-      <c r="AB50"/>
-      <c r="AC50"/>
-      <c r="AD50"/>
-      <c r="AE50"/>
+      <c r="Z50" s="6"/>
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>134</v>
+        <v>213</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D51" s="13">
         <v>2</v>
@@ -6010,54 +5982,52 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G51" s="13"/>
+      <c r="G51" s="13">
+        <v>38</v>
+      </c>
       <c r="H51" s="13">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I51" s="13">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J51" s="13"/>
       <c r="K51" s="21"/>
       <c r="L51" s="12">
         <v>1</v>
       </c>
-      <c r="M51" s="12">
-        <v>0</v>
-      </c>
+      <c r="M51" s="12"/>
       <c r="N51" s="35"/>
-      <c r="O51" s="35">
-        <v>0</v>
-      </c>
+      <c r="O51" s="35"/>
       <c r="P51" s="84">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Q51" s="84">
-        <v>0.5</v>
-      </c>
-      <c r="R51" s="84"/>
-      <c r="S51" s="84">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R51" s="84">
+        <v>1</v>
+      </c>
+      <c r="S51" s="84"/>
       <c r="T51" s="84">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U51" s="84">
         <v>1</v>
       </c>
       <c r="V51" s="75">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="W51" s="33"/>
     </row>
     <row r="52" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D52" s="14">
         <v>3</v>
@@ -6070,52 +6040,46 @@
         <v>4</v>
       </c>
       <c r="G52" s="14">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="H52" s="14">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I52" s="14">
-        <v>6</v>
-      </c>
-      <c r="J52" s="14">
-        <v>30</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J52" s="14"/>
       <c r="K52" s="22"/>
       <c r="L52" s="2">
         <v>1</v>
       </c>
-      <c r="M52" s="20">
-        <v>0</v>
-      </c>
-      <c r="N52" s="34">
-        <v>0</v>
-      </c>
-      <c r="O52" s="81">
-        <v>0</v>
-      </c>
+      <c r="M52" s="20"/>
+      <c r="N52" s="34"/>
+      <c r="O52" s="34"/>
       <c r="P52" s="83">
         <v>1</v>
       </c>
       <c r="Q52" s="83">
-        <v>0.25</v>
-      </c>
-      <c r="R52" s="83"/>
-      <c r="S52" s="83">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="R52" s="83">
+        <v>1</v>
+      </c>
+      <c r="S52" s="83"/>
       <c r="T52" s="83">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="U52" s="83">
         <v>1</v>
       </c>
-      <c r="V52" s="75">
+      <c r="V52" s="89">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="W52" s="33"/>
-      <c r="X52" s="15"/>
+      <c r="X52" s="3"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
       <c r="AA52"/>
       <c r="AB52"/>
       <c r="AC52"/>
@@ -6123,65 +6087,73 @@
       <c r="AE52"/>
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B53" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="D53" s="14">
-        <v>3</v>
-      </c>
-      <c r="E53" s="14">
-        <v>0</v>
-      </c>
-      <c r="F53" s="14">
+      <c r="A53" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="13">
+        <v>2</v>
+      </c>
+      <c r="E53" s="13">
+        <v>0</v>
+      </c>
+      <c r="F53" s="13">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G53" s="14">
-        <v>4</v>
-      </c>
-      <c r="I53" s="14">
         <v>2</v>
       </c>
-      <c r="J53" s="14">
-        <v>31</v>
-      </c>
-      <c r="K53" s="22"/>
-      <c r="L53" s="2">
-        <v>1</v>
-      </c>
-      <c r="M53" s="20">
-        <v>0</v>
-      </c>
-      <c r="N53" s="34">
-        <v>0</v>
-      </c>
-      <c r="O53" s="81">
-        <v>0</v>
-      </c>
-      <c r="P53" s="83">
-        <v>0</v>
-      </c>
-      <c r="S53" s="83">
-        <v>1</v>
-      </c>
-      <c r="U53" s="83">
+      <c r="G53" s="13"/>
+      <c r="H53" s="13">
+        <v>33</v>
+      </c>
+      <c r="I53" s="13">
+        <v>1</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="12">
+        <v>1</v>
+      </c>
+      <c r="M53" s="12">
+        <v>0</v>
+      </c>
+      <c r="N53" s="35"/>
+      <c r="O53" s="35">
+        <v>0</v>
+      </c>
+      <c r="P53" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="Q53" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="R53" s="84"/>
+      <c r="S53" s="84">
+        <v>1</v>
+      </c>
+      <c r="T53" s="84">
+        <v>0.5</v>
+      </c>
+      <c r="U53" s="84">
         <v>1</v>
       </c>
       <c r="V53" s="75">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W53" s="33"/>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
       <c r="B54" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D54" s="14">
         <v>3</v>
@@ -6194,7 +6166,16 @@
         <v>4</v>
       </c>
       <c r="G54" s="14">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="H54" s="14">
+        <v>34</v>
+      </c>
+      <c r="I54" s="14">
+        <v>6</v>
+      </c>
+      <c r="J54" s="14">
+        <v>30</v>
       </c>
       <c r="K54" s="22"/>
       <c r="L54" s="2">
@@ -6203,198 +6184,188 @@
       <c r="M54" s="20">
         <v>0</v>
       </c>
-      <c r="N54" s="34"/>
+      <c r="N54" s="34">
+        <v>0</v>
+      </c>
       <c r="O54" s="81">
         <v>0</v>
       </c>
       <c r="P54" s="83">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q54" s="83">
+        <v>0.25</v>
+      </c>
+      <c r="R54" s="83"/>
+      <c r="S54" s="83">
+        <v>1</v>
+      </c>
+      <c r="T54" s="83">
+        <v>0.25</v>
       </c>
       <c r="U54" s="83">
         <v>1</v>
       </c>
       <c r="V54" s="75">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="W54" s="33"/>
-      <c r="AB54" s="33"/>
-      <c r="AC54" s="6"/>
-      <c r="AD54" s="6"/>
-      <c r="AE54" s="6"/>
+      <c r="X54" s="15"/>
+      <c r="AA54"/>
+      <c r="AB54"/>
+      <c r="AC54"/>
+      <c r="AD54"/>
+      <c r="AE54"/>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B55" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D55" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E55" s="14">
         <v>0</v>
       </c>
       <c r="F55" s="14">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G55" s="14">
+        <v>4</v>
+      </c>
+      <c r="I55" s="14">
         <v>2</v>
       </c>
-      <c r="G55" s="14">
-        <v>6</v>
-      </c>
-      <c r="I55" s="14">
-        <v>3</v>
-      </c>
       <c r="J55" s="14">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K55" s="22"/>
       <c r="L55" s="2">
         <v>1</v>
       </c>
       <c r="M55" s="20">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N55" s="34">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O55" s="81">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="P55" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q55" s="83">
-        <v>0.5</v>
-      </c>
-      <c r="R55" s="83">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="S55" s="83">
         <v>1</v>
-      </c>
-      <c r="T55" s="83">
-        <v>0.5</v>
       </c>
       <c r="U55" s="83">
         <v>1</v>
       </c>
       <c r="V55" s="75">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W55" s="33"/>
-      <c r="AB55" s="33"/>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D56" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E56" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G56" s="14">
-        <v>8</v>
-      </c>
-      <c r="H56" s="14">
-        <v>35</v>
-      </c>
-      <c r="I56" s="14">
-        <v>4</v>
-      </c>
-      <c r="J56" s="14">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="K56" s="22"/>
+      <c r="L56" s="2">
+        <v>1</v>
+      </c>
       <c r="M56" s="20">
-        <v>1</v>
-      </c>
-      <c r="N56" s="34">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N56" s="34"/>
       <c r="O56" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P56" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q56" s="83">
-        <v>1</v>
-      </c>
-      <c r="R56" s="83">
-        <v>1</v>
-      </c>
-      <c r="S56" s="83">
-        <v>1</v>
-      </c>
-      <c r="T56" s="83">
+        <v>0</v>
+      </c>
+      <c r="U56" s="83">
         <v>1</v>
       </c>
       <c r="V56" s="75">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W56" s="33"/>
       <c r="AB56" s="33"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="6"/>
+      <c r="AE56" s="6"/>
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D57" s="14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E57" s="14">
         <v>0</v>
       </c>
       <c r="F57" s="14">
         <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G57" s="14">
         <v>6</v>
       </c>
-      <c r="G57" s="14">
-        <v>9</v>
-      </c>
-      <c r="H57" s="14">
-        <v>36</v>
-      </c>
       <c r="I57" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J57" s="14">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K57" s="22"/>
+      <c r="L57" s="2">
+        <v>1</v>
+      </c>
       <c r="M57" s="20">
         <v>0.2</v>
       </c>
       <c r="N57" s="34">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O57" s="81">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="P57" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q57" s="83">
         <v>0.5</v>
       </c>
       <c r="R57" s="83">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S57" s="83">
         <v>1</v>
@@ -6402,43 +6373,46 @@
       <c r="T57" s="83">
         <v>0.5</v>
       </c>
+      <c r="U57" s="83">
+        <v>1</v>
+      </c>
       <c r="V57" s="75">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="W57" s="33"/>
-      <c r="Z57" s="6"/>
       <c r="AB57" s="33"/>
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D58" s="14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E58" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="G58" s="14">
+        <v>8</v>
       </c>
       <c r="H58" s="14">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="I58" s="14">
+        <v>4</v>
       </c>
       <c r="J58" s="14">
-        <v>35</v>
-      </c>
-      <c r="K58" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="L58" s="2">
-        <v>1</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="K58" s="22"/>
       <c r="M58" s="20">
         <v>1</v>
       </c>
@@ -6449,7 +6423,7 @@
         <v>1</v>
       </c>
       <c r="P58" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q58" s="83">
         <v>1</v>
@@ -6461,87 +6435,105 @@
         <v>1</v>
       </c>
       <c r="T58" s="83">
-        <v>1</v>
-      </c>
-      <c r="U58" s="83">
         <v>1</v>
       </c>
       <c r="V58" s="75">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W58" s="33"/>
       <c r="AB58" s="33"/>
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D59" s="14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E59" s="14">
         <v>0</v>
       </c>
       <c r="F59" s="14">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="G59" s="14">
+        <v>9</v>
+      </c>
+      <c r="H59" s="14">
+        <v>36</v>
+      </c>
+      <c r="I59" s="14">
+        <v>5</v>
       </c>
       <c r="J59" s="14">
-        <v>36</v>
-      </c>
-      <c r="K59" s="22" t="s">
-        <v>194</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="K59" s="22"/>
       <c r="M59" s="20">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="N59" s="34">
         <v>1</v>
       </c>
-      <c r="O59" s="33"/>
+      <c r="O59" s="81">
+        <v>1</v>
+      </c>
       <c r="P59" s="83">
         <v>0</v>
       </c>
       <c r="Q59" s="83">
         <v>0.5</v>
       </c>
+      <c r="R59" s="83">
+        <v>1</v>
+      </c>
+      <c r="S59" s="83">
+        <v>1</v>
+      </c>
       <c r="T59" s="83">
         <v>0.5</v>
       </c>
       <c r="V59" s="75">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="W59" s="33"/>
-      <c r="AA59" s="6"/>
+      <c r="Z59" s="6"/>
       <c r="AB59" s="33"/>
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D60" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="14">
         <v>0</v>
       </c>
       <c r="F60" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="H60" s="14">
+        <v>37</v>
       </c>
       <c r="J60" s="14">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K60" s="22" t="s">
-        <v>92</v>
+        <v>192</v>
+      </c>
+      <c r="L60" s="2">
+        <v>1</v>
       </c>
       <c r="M60" s="20">
         <v>1</v>
@@ -6549,372 +6541,394 @@
       <c r="N60" s="34">
         <v>1</v>
       </c>
-      <c r="O60" s="34">
-        <v>0.5</v>
+      <c r="O60" s="81">
+        <v>1</v>
       </c>
       <c r="P60" s="83">
         <v>0</v>
       </c>
       <c r="Q60" s="83">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="R60" s="83">
+        <v>1</v>
+      </c>
+      <c r="S60" s="83">
+        <v>1</v>
       </c>
       <c r="T60" s="83">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="U60" s="83">
+        <v>1</v>
       </c>
       <c r="V60" s="75">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="W60" s="33"/>
       <c r="AB60" s="33"/>
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="C61" s="31" t="s">
         <v>211</v>
       </c>
       <c r="D61" s="14">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E61" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F61" s="14">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G61" s="14">
-        <v>10</v>
-      </c>
-      <c r="K61" s="22"/>
+        <v>4</v>
+      </c>
+      <c r="J61" s="14">
+        <v>36</v>
+      </c>
+      <c r="K61" s="22" t="s">
+        <v>193</v>
+      </c>
       <c r="M61" s="20">
-        <v>0</v>
-      </c>
-      <c r="N61" s="34"/>
+        <v>0.5</v>
+      </c>
+      <c r="N61" s="34">
+        <v>1</v>
+      </c>
       <c r="O61" s="33"/>
       <c r="P61" s="83">
         <v>0</v>
       </c>
-      <c r="S61" s="83">
-        <v>1</v>
+      <c r="Q61" s="83">
+        <v>0.5</v>
+      </c>
+      <c r="T61" s="83">
+        <v>0.5</v>
       </c>
       <c r="V61" s="75">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="W61" s="33"/>
+      <c r="AA61" s="6"/>
       <c r="AB61" s="33"/>
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D62" s="14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E62" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="G62" s="14">
-        <v>11</v>
-      </c>
-      <c r="K62" s="22"/>
-      <c r="N62" s="34"/>
-      <c r="O62" s="33"/>
+        <v>6</v>
+      </c>
+      <c r="J62" s="14">
+        <v>37</v>
+      </c>
+      <c r="K62" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="M62" s="20">
+        <v>1</v>
+      </c>
+      <c r="N62" s="34">
+        <v>1</v>
+      </c>
+      <c r="O62" s="34">
+        <v>0.5</v>
+      </c>
       <c r="P62" s="83">
         <v>0</v>
       </c>
       <c r="Q62" s="83">
-        <v>0</v>
-      </c>
-      <c r="S62" s="83">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="T62" s="83">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="V62" s="75">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="W62" s="33"/>
       <c r="AB62" s="33"/>
-      <c r="AC62" s="6"/>
-      <c r="AD62" s="6"/>
-      <c r="AE62" s="6"/>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B63" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D63" s="14">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E63" s="14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="14">
         <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G63" s="14">
+        <v>10</v>
+      </c>
+      <c r="K63" s="22"/>
+      <c r="M63" s="20">
+        <v>0</v>
+      </c>
+      <c r="N63" s="34"/>
+      <c r="O63" s="33"/>
+      <c r="P63" s="83">
+        <v>0</v>
+      </c>
+      <c r="S63" s="83">
+        <v>1</v>
+      </c>
+      <c r="V63" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="W63" s="33"/>
+      <c r="AB63" s="33"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B64" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" s="14">
+        <v>7</v>
+      </c>
+      <c r="E64" s="14">
+        <v>1</v>
+      </c>
+      <c r="F64" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G64" s="14">
+        <v>11</v>
+      </c>
+      <c r="K64" s="22"/>
+      <c r="N64" s="34"/>
+      <c r="O64" s="33"/>
+      <c r="P64" s="83">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="83">
+        <v>0</v>
+      </c>
+      <c r="S64" s="83">
+        <v>1</v>
+      </c>
+      <c r="T64" s="83">
+        <v>0</v>
+      </c>
+      <c r="V64" s="75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="W64" s="33"/>
+      <c r="AB64" s="33"/>
+      <c r="AC64" s="6"/>
+      <c r="AD64" s="6"/>
+      <c r="AE64" s="6"/>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B65" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" s="14">
+        <v>5</v>
+      </c>
+      <c r="E65" s="14">
+        <v>0</v>
+      </c>
+      <c r="F65" s="14">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J63" s="14">
+      <c r="J65" s="14">
         <v>38</v>
       </c>
-      <c r="K63" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="M63" s="20">
-        <v>1</v>
-      </c>
-      <c r="N63" s="34">
-        <v>1</v>
-      </c>
-      <c r="O63" s="34"/>
-      <c r="P63" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="83">
+      <c r="K65" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="M65" s="20">
+        <v>1</v>
+      </c>
+      <c r="N65" s="34">
+        <v>1</v>
+      </c>
+      <c r="O65" s="34"/>
+      <c r="P65" s="83">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="83">
         <v>0.5</v>
       </c>
-      <c r="T63" s="83">
+      <c r="T65" s="83">
         <v>0.5</v>
       </c>
-      <c r="V63" s="89">
+      <c r="V65" s="89">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="W63" s="33"/>
-      <c r="AA63" s="6"/>
-      <c r="AB63" s="33"/>
-    </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
+      <c r="W65" s="33"/>
+      <c r="AA65" s="6"/>
+      <c r="AB65" s="33"/>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C64" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="D64" s="13">
+      <c r="B66" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D66" s="13">
         <v>3</v>
       </c>
-      <c r="E64" s="13">
-        <v>0</v>
-      </c>
-      <c r="F64" s="13">
+      <c r="E66" s="13">
+        <v>0</v>
+      </c>
+      <c r="F66" s="13">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G64" s="13">
+      <c r="G66" s="13">
         <v>45</v>
       </c>
-      <c r="H64" s="13">
+      <c r="H66" s="13">
         <v>27</v>
       </c>
-      <c r="I64" s="13">
+      <c r="I66" s="13">
         <v>36</v>
       </c>
-      <c r="J64" s="13">
+      <c r="J66" s="13">
         <v>29</v>
       </c>
-      <c r="K64" s="21"/>
-      <c r="L64" s="12">
-        <v>1</v>
-      </c>
-      <c r="M64" s="12">
+      <c r="K66" s="21"/>
+      <c r="L66" s="12">
+        <v>1</v>
+      </c>
+      <c r="M66" s="12">
         <v>0.5</v>
       </c>
-      <c r="N64" s="35"/>
-      <c r="O64" s="35"/>
-      <c r="P64" s="84">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="84"/>
-      <c r="R64" s="84"/>
-      <c r="S64" s="84">
-        <v>1</v>
-      </c>
-      <c r="T64" s="84">
+      <c r="N66" s="35"/>
+      <c r="O66" s="35"/>
+      <c r="P66" s="84">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="84"/>
+      <c r="R66" s="84"/>
+      <c r="S66" s="84">
+        <v>1</v>
+      </c>
+      <c r="T66" s="84">
         <v>0.5</v>
       </c>
-      <c r="U64" s="84"/>
-      <c r="V64" s="75">
+      <c r="U66" s="84"/>
+      <c r="V66" s="75">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="W64" s="33"/>
-      <c r="AB64" s="33"/>
-    </row>
-    <row r="65" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="10"/>
-      <c r="B65" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="C65" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="D65" s="14">
+      <c r="W66" s="33"/>
+      <c r="AB66" s="33"/>
+    </row>
+    <row r="67" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+      <c r="B67" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D67" s="14">
         <v>7</v>
       </c>
-      <c r="E65" s="14">
+      <c r="E67" s="14">
         <v>2</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F67" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G67" s="14">
         <v>46</v>
       </c>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="20"/>
-      <c r="N65" s="34"/>
-      <c r="O65" s="33"/>
-      <c r="P65" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="83"/>
-      <c r="R65" s="83"/>
-      <c r="S65" s="83">
-        <v>1</v>
-      </c>
-      <c r="T65" s="83"/>
-      <c r="U65" s="83"/>
-      <c r="V65" s="75">
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="2"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="34"/>
+      <c r="O67" s="33"/>
+      <c r="P67" s="83">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="83"/>
+      <c r="R67" s="83"/>
+      <c r="S67" s="83">
+        <v>1</v>
+      </c>
+      <c r="T67" s="83"/>
+      <c r="U67" s="83"/>
+      <c r="V67" s="75">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="W65" s="33"/>
-      <c r="X65" s="3"/>
-      <c r="Y65"/>
-      <c r="Z65"/>
-      <c r="AA65"/>
-      <c r="AB65" s="33"/>
-      <c r="AC65"/>
-      <c r="AD65"/>
-      <c r="AE65"/>
-    </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B66" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="C66" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="D66" s="14">
+      <c r="W67" s="33"/>
+      <c r="X67" s="3"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+      <c r="AA67"/>
+      <c r="AB67" s="33"/>
+      <c r="AC67"/>
+      <c r="AD67"/>
+      <c r="AE67"/>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B68" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C68" s="31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" s="14">
         <v>7</v>
       </c>
-      <c r="E66" s="14">
+      <c r="E68" s="14">
         <v>2</v>
       </c>
-      <c r="F66" s="14">
+      <c r="F68" s="14">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G66" s="14">
+      <c r="G68" s="14">
         <v>47</v>
       </c>
-      <c r="K66" s="22"/>
-      <c r="N66" s="34"/>
-      <c r="O66" s="33"/>
-      <c r="P66" s="83">
-        <v>0</v>
-      </c>
-      <c r="V66" s="75">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="W66" s="33"/>
-    </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A67" s="48"/>
-      <c r="B67" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="D67" s="27">
-        <v>10</v>
-      </c>
-      <c r="E67" s="27">
-        <v>0</v>
-      </c>
-      <c r="F67" s="27">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="G67" s="27">
-        <v>34</v>
-      </c>
-      <c r="H67" s="27"/>
-      <c r="I67" s="27"/>
-      <c r="J67" s="27"/>
-      <c r="K67" s="29"/>
-      <c r="L67" s="37"/>
-      <c r="M67" s="37"/>
-      <c r="N67" s="37"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="86">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="86"/>
-      <c r="R67" s="86"/>
-      <c r="S67" s="86">
-        <v>1</v>
-      </c>
-      <c r="T67" s="86"/>
-      <c r="U67" s="86"/>
-      <c r="V67" s="89">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="W67" s="33"/>
-    </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A68" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="D68" s="14">
-        <v>4</v>
-      </c>
-      <c r="E68" s="14">
-        <v>0</v>
-      </c>
-      <c r="F68" s="14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G68" s="14">
-        <v>48</v>
-      </c>
-      <c r="K68" s="22" t="s">
-        <v>198</v>
-      </c>
+      <c r="K68" s="22"/>
       <c r="N68" s="34"/>
       <c r="O68" s="33"/>
       <c r="P68" s="83">
@@ -6925,66 +6939,61 @@
         <v>0</v>
       </c>
       <c r="W68" s="33"/>
-      <c r="Y68" s="33"/>
-      <c r="AA68" s="6"/>
-    </row>
-    <row r="69" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="10"/>
-      <c r="B69" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="31" t="s">
-        <v>211</v>
-      </c>
-      <c r="D69" s="14">
-        <v>3</v>
-      </c>
-      <c r="E69" s="14">
-        <v>0</v>
-      </c>
-      <c r="F69" s="14">
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A69" s="48"/>
+      <c r="B69" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D69" s="27">
+        <v>10</v>
+      </c>
+      <c r="E69" s="27">
+        <v>0</v>
+      </c>
+      <c r="F69" s="27">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="G69" s="14">
-        <v>49</v>
-      </c>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="2"/>
-      <c r="M69" s="20"/>
-      <c r="N69" s="34"/>
-      <c r="O69" s="34"/>
-      <c r="P69" s="83">
-        <v>0</v>
-      </c>
-      <c r="Q69" s="83"/>
-      <c r="R69" s="83"/>
-      <c r="S69" s="83"/>
-      <c r="T69" s="83"/>
-      <c r="U69" s="83"/>
-      <c r="V69" s="75">
+        <v>10</v>
+      </c>
+      <c r="G69" s="27">
+        <v>34</v>
+      </c>
+      <c r="H69" s="27"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37"/>
+      <c r="O69" s="37"/>
+      <c r="P69" s="86">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="86"/>
+      <c r="R69" s="86"/>
+      <c r="S69" s="86">
+        <v>1</v>
+      </c>
+      <c r="T69" s="86"/>
+      <c r="U69" s="86"/>
+      <c r="V69" s="89">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W69" s="33"/>
-      <c r="X69" s="3"/>
-      <c r="Y69"/>
-      <c r="Z69"/>
-      <c r="AA69"/>
-      <c r="AB69"/>
-      <c r="AC69"/>
-      <c r="AD69"/>
-      <c r="AE69"/>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A70" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="B70" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>210</v>
+        <v>149</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>209</v>
       </c>
       <c r="D70" s="14">
         <v>4</v>
@@ -6996,79 +7005,67 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="G70" s="14">
+        <v>48</v>
+      </c>
       <c r="K70" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="L70" s="83"/>
-      <c r="M70" s="85"/>
-      <c r="N70" s="83"/>
-      <c r="O70" s="83"/>
+        <v>197</v>
+      </c>
+      <c r="N70" s="34"/>
+      <c r="O70" s="33"/>
       <c r="P70" s="83">
-        <v>1</v>
-      </c>
-      <c r="V70" s="89">
+        <v>0</v>
+      </c>
+      <c r="V70" s="75">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W70" s="33"/>
-      <c r="AB70" s="6"/>
-      <c r="AC70" s="6"/>
-      <c r="AD70" s="6"/>
-      <c r="AE70" s="6"/>
-    </row>
-    <row r="71" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B71" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="13">
-        <v>2</v>
-      </c>
-      <c r="E71" s="13">
-        <v>0</v>
-      </c>
-      <c r="F71" s="13">
+      <c r="Y70" s="33"/>
+      <c r="AA70" s="6"/>
+    </row>
+    <row r="71" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="10"/>
+      <c r="B71" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>210</v>
+      </c>
+      <c r="D71" s="14">
+        <v>3</v>
+      </c>
+      <c r="E71" s="14">
+        <v>0</v>
+      </c>
+      <c r="F71" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="12">
-        <v>1</v>
-      </c>
-      <c r="M71" s="12">
-        <v>0.8</v>
-      </c>
-      <c r="N71" s="35">
-        <v>1</v>
-      </c>
-      <c r="O71" s="35">
-        <v>1</v>
-      </c>
-      <c r="P71" s="84">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="84">
-        <v>1</v>
-      </c>
-      <c r="R71" s="84">
-        <v>1</v>
-      </c>
-      <c r="S71" s="84"/>
-      <c r="T71" s="84">
-        <v>1</v>
-      </c>
-      <c r="U71" s="84"/>
+        <v>4</v>
+      </c>
+      <c r="G71" s="14">
+        <v>49</v>
+      </c>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="22"/>
+      <c r="L71" s="2"/>
+      <c r="M71" s="20"/>
+      <c r="N71" s="34"/>
+      <c r="O71" s="34"/>
+      <c r="P71" s="83">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="83"/>
+      <c r="R71" s="83"/>
+      <c r="S71" s="83"/>
+      <c r="T71" s="83"/>
+      <c r="U71" s="83"/>
       <c r="V71" s="75">
-        <f t="shared" ref="V71:V79" si="3">SUM(R71:U71)</f>
-        <v>2</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W71" s="33"/>
       <c r="X71" s="3"/>
       <c r="Y71"/>
       <c r="Z71"/>
@@ -7079,147 +7076,159 @@
       <c r="AE71"/>
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A72" s="30"/>
-      <c r="B72" s="31" t="s">
+      <c r="B72" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" s="14">
+        <v>4</v>
+      </c>
+      <c r="E72" s="14">
+        <v>0</v>
+      </c>
+      <c r="F72" s="14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K72" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="L72" s="83"/>
+      <c r="M72" s="85"/>
+      <c r="N72" s="83"/>
+      <c r="O72" s="83"/>
+      <c r="P72" s="83">
+        <v>1</v>
+      </c>
+      <c r="V72" s="89">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W72" s="33"/>
+      <c r="AB72" s="6"/>
+      <c r="AC72" s="6"/>
+      <c r="AD72" s="6"/>
+      <c r="AE72" s="6"/>
+    </row>
+    <row r="73" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C73" s="26"/>
+      <c r="D73" s="13">
+        <v>2</v>
+      </c>
+      <c r="E73" s="13">
+        <v>0</v>
+      </c>
+      <c r="F73" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="12">
+        <v>1</v>
+      </c>
+      <c r="M73" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="N73" s="35">
+        <v>1</v>
+      </c>
+      <c r="O73" s="35">
+        <v>1</v>
+      </c>
+      <c r="P73" s="84">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="84">
+        <v>1</v>
+      </c>
+      <c r="R73" s="84">
+        <v>1</v>
+      </c>
+      <c r="S73" s="84"/>
+      <c r="T73" s="84">
+        <v>1</v>
+      </c>
+      <c r="U73" s="84"/>
+      <c r="V73" s="75">
+        <f t="shared" ref="V73:V81" si="3">SUM(R73:U73)</f>
+        <v>2</v>
+      </c>
+      <c r="X73" s="3"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+      <c r="AA73"/>
+      <c r="AB73"/>
+      <c r="AC73"/>
+      <c r="AD73"/>
+      <c r="AE73"/>
+    </row>
+    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A74" s="30"/>
+      <c r="B74" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="31"/>
-      <c r="D72" s="14">
+      <c r="C74" s="31"/>
+      <c r="D74" s="14">
         <v>2</v>
       </c>
-      <c r="E72" s="14">
-        <v>1</v>
-      </c>
-      <c r="F72" s="14">
-        <f t="shared" ref="F72:F79" si="4">CEILING(D72,X$22+1)</f>
+      <c r="E74" s="14">
+        <v>1</v>
+      </c>
+      <c r="F74" s="14">
+        <f t="shared" ref="F74:F81" si="4">CEILING(D74,X$22+1)</f>
         <v>2</v>
       </c>
-      <c r="K72" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="L72" s="20"/>
-      <c r="N72" s="36"/>
-      <c r="O72" s="36">
-        <v>1</v>
-      </c>
-      <c r="P72" s="85">
-        <v>1</v>
-      </c>
-      <c r="Q72" s="85">
-        <v>1</v>
-      </c>
-      <c r="R72" s="85">
-        <v>1</v>
-      </c>
-      <c r="S72" s="85"/>
-      <c r="T72" s="85">
-        <v>1</v>
-      </c>
-      <c r="U72" s="85"/>
-      <c r="V72" s="75">
+      <c r="K74" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="L74" s="20"/>
+      <c r="N74" s="36"/>
+      <c r="O74" s="36">
+        <v>1</v>
+      </c>
+      <c r="P74" s="85">
+        <v>1</v>
+      </c>
+      <c r="Q74" s="85">
+        <v>1</v>
+      </c>
+      <c r="R74" s="85">
+        <v>1</v>
+      </c>
+      <c r="S74" s="85"/>
+      <c r="T74" s="85">
+        <v>1</v>
+      </c>
+      <c r="U74" s="85"/>
+      <c r="V74" s="75">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="W72" s="33"/>
-    </row>
-    <row r="73" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="30"/>
-      <c r="B73" s="31" t="s">
-        <v>227</v>
-      </c>
-      <c r="C73" s="31"/>
-      <c r="D73" s="14">
-        <v>1</v>
-      </c>
-      <c r="E73" s="14">
-        <v>1</v>
-      </c>
-      <c r="F73" s="14">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="22" t="s">
-        <v>228</v>
-      </c>
-      <c r="L73" s="85"/>
-      <c r="M73" s="85"/>
-      <c r="N73" s="85"/>
-      <c r="O73" s="85"/>
-      <c r="P73" s="85"/>
-      <c r="Q73" s="85"/>
-      <c r="R73" s="85"/>
-      <c r="S73" s="85"/>
-      <c r="T73" s="85"/>
-      <c r="U73" s="85"/>
-      <c r="V73" s="75"/>
-      <c r="X73" s="3"/>
-    </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="B74" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="14">
-        <v>4</v>
-      </c>
-      <c r="E74" s="14">
-        <v>3</v>
-      </c>
-      <c r="F74" s="14">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="K74" s="22"/>
-      <c r="L74" s="2">
-        <v>1</v>
-      </c>
-      <c r="M74" s="20">
-        <v>1</v>
-      </c>
-      <c r="N74" s="34">
-        <v>1</v>
-      </c>
-      <c r="O74" s="81">
-        <v>1</v>
-      </c>
-      <c r="P74" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="83">
-        <v>1</v>
-      </c>
-      <c r="R74" s="83">
-        <v>1</v>
-      </c>
-      <c r="T74" s="83">
-        <v>1</v>
-      </c>
-      <c r="U74" s="83">
-        <v>1</v>
-      </c>
-      <c r="V74" s="75">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
       <c r="W74" s="33"/>
-      <c r="Y74" s="33"/>
-      <c r="Z74" s="33"/>
-      <c r="AA74" s="33"/>
-    </row>
-    <row r="75" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="10"/>
-      <c r="B75" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C75" s="23"/>
+    </row>
+    <row r="75" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="30"/>
+      <c r="B75" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C75" s="31"/>
       <c r="D75" s="14">
         <v>1</v>
       </c>
       <c r="E75" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F75" s="14">
         <f t="shared" si="4"/>
@@ -7230,79 +7239,78 @@
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
       <c r="K75" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="L75" s="2"/>
-      <c r="M75" s="20">
-        <v>1</v>
-      </c>
-      <c r="N75" s="34">
-        <v>1</v>
-      </c>
-      <c r="O75" s="81">
-        <v>1</v>
-      </c>
-      <c r="P75" s="83">
-        <v>1</v>
-      </c>
-      <c r="Q75" s="83">
-        <v>1</v>
-      </c>
-      <c r="R75" s="83">
-        <v>1</v>
-      </c>
-      <c r="S75" s="83"/>
-      <c r="T75" s="83">
-        <v>1</v>
-      </c>
-      <c r="U75" s="83"/>
-      <c r="V75" s="75">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="W75" s="15"/>
+        <v>227</v>
+      </c>
+      <c r="L75" s="85"/>
+      <c r="M75" s="85"/>
+      <c r="N75" s="85"/>
+      <c r="O75" s="85"/>
+      <c r="P75" s="85"/>
+      <c r="Q75" s="85"/>
+      <c r="R75" s="85"/>
+      <c r="S75" s="85"/>
+      <c r="T75" s="85"/>
+      <c r="U75" s="85"/>
+      <c r="V75" s="75"/>
       <c r="X75" s="3"/>
-      <c r="Y75"/>
-      <c r="Z75" s="33"/>
-      <c r="AA75"/>
-      <c r="AB75" s="33"/>
-      <c r="AC75" s="33"/>
-      <c r="AD75" s="33"/>
-      <c r="AE75" s="33"/>
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B76" s="23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D76" s="14">
+        <v>4</v>
+      </c>
+      <c r="E76" s="14">
         <v>3</v>
-      </c>
-      <c r="E76" s="14">
-        <v>1</v>
       </c>
       <c r="F76" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K76" s="22"/>
-      <c r="N76" s="34"/>
-      <c r="O76" s="33"/>
-      <c r="P76" s="33"/>
-      <c r="Q76" s="33"/>
-      <c r="R76" s="33"/>
-      <c r="S76" s="33"/>
-      <c r="T76" s="33"/>
-      <c r="U76" s="33"/>
+      <c r="L76" s="2">
+        <v>1</v>
+      </c>
+      <c r="M76" s="20">
+        <v>1</v>
+      </c>
+      <c r="N76" s="34">
+        <v>1</v>
+      </c>
+      <c r="O76" s="81">
+        <v>1</v>
+      </c>
+      <c r="P76" s="83">
+        <v>1</v>
+      </c>
+      <c r="Q76" s="83">
+        <v>1</v>
+      </c>
+      <c r="R76" s="83">
+        <v>1</v>
+      </c>
+      <c r="T76" s="83">
+        <v>1</v>
+      </c>
+      <c r="U76" s="83">
+        <v>1</v>
+      </c>
       <c r="V76" s="75">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W76" s="15"/>
-    </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="W76" s="33"/>
+      <c r="Y76" s="33"/>
+      <c r="Z76" s="33"/>
+      <c r="AA76" s="33"/>
+    </row>
+    <row r="77" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="10"/>
       <c r="B77" s="23" t="s">
-        <v>156</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="C77" s="23"/>
       <c r="D77" s="14">
         <v>1</v>
       </c>
@@ -7313,43 +7321,67 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="K77" s="22"/>
-      <c r="N77" s="34"/>
-      <c r="O77" s="33"/>
-      <c r="P77" s="33"/>
-      <c r="Q77" s="33"/>
-      <c r="R77" s="33"/>
-      <c r="S77" s="33"/>
-      <c r="T77" s="33"/>
-      <c r="U77" s="33"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="L77" s="2"/>
+      <c r="M77" s="20">
+        <v>1</v>
+      </c>
+      <c r="N77" s="34">
+        <v>1</v>
+      </c>
+      <c r="O77" s="81">
+        <v>1</v>
+      </c>
+      <c r="P77" s="83">
+        <v>1</v>
+      </c>
+      <c r="Q77" s="83">
+        <v>1</v>
+      </c>
+      <c r="R77" s="83">
+        <v>1</v>
+      </c>
+      <c r="S77" s="83"/>
+      <c r="T77" s="83">
+        <v>1</v>
+      </c>
+      <c r="U77" s="83"/>
       <c r="V77" s="75">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W77" s="15"/>
-      <c r="AB77" s="6"/>
-      <c r="AC77" s="6"/>
-      <c r="AD77" s="6"/>
-      <c r="AE77" s="6"/>
+      <c r="X77" s="3"/>
+      <c r="Y77"/>
+      <c r="Z77" s="33"/>
+      <c r="AA77"/>
+      <c r="AB77" s="33"/>
+      <c r="AC77" s="33"/>
+      <c r="AD77" s="33"/>
+      <c r="AE77" s="33"/>
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B78" s="23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D78" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E78" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="14">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="K78" s="22"/>
-      <c r="L78" s="83"/>
-      <c r="M78" s="85"/>
-      <c r="N78" s="83"/>
+      <c r="N78" s="34"/>
       <c r="O78" s="33"/>
       <c r="P78" s="33"/>
       <c r="Q78" s="33"/>
@@ -7363,343 +7395,407 @@
       </c>
       <c r="W78" s="15"/>
     </row>
-    <row r="79" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="10"/>
-      <c r="B79" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C79" s="24"/>
-      <c r="D79" s="27">
-        <v>1</v>
-      </c>
-      <c r="E79" s="27">
-        <v>0</v>
-      </c>
-      <c r="F79" s="27">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B79" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D79" s="14">
+        <v>1</v>
+      </c>
+      <c r="E79" s="14">
+        <v>0</v>
+      </c>
+      <c r="F79" s="14">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G79" s="27"/>
-      <c r="H79" s="27"/>
-      <c r="I79" s="27"/>
-      <c r="J79" s="27"/>
-      <c r="K79" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="L79" s="28"/>
-      <c r="M79" s="28">
-        <v>1</v>
-      </c>
-      <c r="N79" s="37"/>
-      <c r="O79" s="37">
-        <v>1</v>
-      </c>
-      <c r="P79" s="37">
-        <v>1</v>
-      </c>
-      <c r="Q79" s="86">
-        <v>1</v>
-      </c>
-      <c r="R79" s="86"/>
-      <c r="S79" s="86">
-        <v>1</v>
-      </c>
-      <c r="T79" s="86">
-        <v>1</v>
-      </c>
-      <c r="U79" s="86"/>
-      <c r="V79" s="89">
+      <c r="K79" s="22"/>
+      <c r="N79" s="34"/>
+      <c r="O79" s="33"/>
+      <c r="P79" s="33"/>
+      <c r="Q79" s="33"/>
+      <c r="R79" s="33"/>
+      <c r="S79" s="33"/>
+      <c r="T79" s="33"/>
+      <c r="U79" s="33"/>
+      <c r="V79" s="75">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W79" s="15"/>
-      <c r="X79" s="3"/>
-      <c r="Y79"/>
-      <c r="Z79"/>
-      <c r="AA79"/>
       <c r="AB79" s="6"/>
       <c r="AC79" s="6"/>
       <c r="AD79" s="6"/>
       <c r="AE79" s="6"/>
     </row>
-    <row r="80" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="11"/>
-    </row>
-    <row r="81" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="K81" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="L81" s="65">
-        <f t="array" ref="L81">SUM($F2:$F79*(L2:L79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>104</v>
-      </c>
-      <c r="M81" s="65">
-        <f t="array" ref="M81">SUM($F2:$F79*(M2:M79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>136</v>
-      </c>
-      <c r="N81" s="65">
-        <f t="array" ref="N81">SUM($F2:$F79*(N2:N79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>144</v>
-      </c>
-      <c r="O81" s="65">
-        <f t="array" ref="O81">SUM($F2:$F79*(O2:O79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>140</v>
-      </c>
-      <c r="P81" s="65">
-        <f t="array" ref="P81">SUM($F2:$F79*(P2:P79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>144</v>
-      </c>
-      <c r="Q81" s="66">
-        <f t="array" ref="Q81">SUM($F2:$F79*(Q2:Q79&gt;=0.9)*($V2:$V79&gt;=$X$12))</f>
-        <v>134</v>
-      </c>
-      <c r="R81" s="68"/>
-      <c r="S81" s="68"/>
-      <c r="T81" s="68"/>
-      <c r="U81" s="68"/>
-      <c r="Y81" s="33"/>
-      <c r="Z81" s="33"/>
-      <c r="AA81" s="33"/>
+    <row r="80" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B80" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D80" s="14">
+        <v>4</v>
+      </c>
+      <c r="E80" s="14">
+        <v>0</v>
+      </c>
+      <c r="F80" s="14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K80" s="22"/>
+      <c r="L80" s="83"/>
+      <c r="M80" s="85"/>
+      <c r="N80" s="83"/>
+      <c r="O80" s="33"/>
+      <c r="P80" s="33"/>
+      <c r="Q80" s="33"/>
+      <c r="R80" s="33"/>
+      <c r="S80" s="33"/>
+      <c r="T80" s="33"/>
+      <c r="U80" s="33"/>
+      <c r="V80" s="75">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W80" s="15"/>
+    </row>
+    <row r="81" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="10"/>
+      <c r="B81" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C81" s="24"/>
+      <c r="D81" s="27">
+        <v>1</v>
+      </c>
+      <c r="E81" s="27">
+        <v>0</v>
+      </c>
+      <c r="F81" s="27">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G81" s="27"/>
+      <c r="H81" s="27"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="L81" s="28"/>
+      <c r="M81" s="28">
+        <v>1</v>
+      </c>
+      <c r="N81" s="37"/>
+      <c r="O81" s="37">
+        <v>1</v>
+      </c>
+      <c r="P81" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="86">
+        <v>1</v>
+      </c>
+      <c r="R81" s="86"/>
+      <c r="S81" s="86">
+        <v>1</v>
+      </c>
+      <c r="T81" s="86">
+        <v>1</v>
+      </c>
+      <c r="U81" s="86"/>
+      <c r="V81" s="89">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="W81" s="15"/>
+      <c r="X81" s="3"/>
+      <c r="Y81"/>
+      <c r="Z81"/>
+      <c r="AA81"/>
       <c r="AB81" s="6"/>
       <c r="AC81" s="6"/>
       <c r="AD81" s="6"/>
       <c r="AE81" s="6"/>
     </row>
-    <row r="82" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="K82" s="67" t="s">
-        <v>167</v>
-      </c>
-      <c r="L82" s="68">
-        <f t="array" ref="L82">SUM($F2:$F79*L2:L79*($V2:$V79&gt;=$X$12))</f>
+    <row r="82" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="11"/>
+    </row>
+    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="K83" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="L83" s="65">
+        <f t="array" ref="L83">SUM($F2:$F81*(L2:L81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
         <v>106</v>
       </c>
-      <c r="M82" s="68">
-        <f t="array" ref="M82">SUM($F2:$F79*M2:M79*($V2:$V79&gt;=$X$12))</f>
-        <v>143.4</v>
-      </c>
-      <c r="N82" s="68">
-        <f t="array" ref="N82">SUM($F2:$F79*N2:N79*($V2:$V79&gt;=$X$12))</f>
-        <v>145</v>
-      </c>
-      <c r="O82" s="68">
-        <f t="array" ref="O82">SUM($F2:$F79*O2:O79*($V2:$V79&gt;=$X$12))</f>
-        <v>151.6</v>
-      </c>
-      <c r="P82" s="68">
-        <f t="array" ref="P82">SUM($F2:$F79*P2:P79*($V2:$V79&gt;=$X$12))</f>
-        <v>149.80000000000001</v>
-      </c>
-      <c r="Q82" s="69">
-        <f t="array" ref="Q82">SUM($F2:$F79*Q2:Q79*($V2:$V79&gt;=$X$12))</f>
-        <v>147</v>
-      </c>
-      <c r="R82" s="68"/>
-      <c r="S82" s="68"/>
-      <c r="T82" s="68"/>
-      <c r="U82" s="68"/>
-      <c r="AB82" s="6"/>
-      <c r="AC82" s="6"/>
-      <c r="AD82" s="6"/>
-      <c r="AE82" s="6"/>
-    </row>
-    <row r="83" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="K83" s="67" t="s">
-        <v>166</v>
-      </c>
-      <c r="L83" s="68">
-        <f t="array" ref="L83">SUM($F$2:$F$79*(L$2:L$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>108</v>
-      </c>
-      <c r="M83" s="68">
-        <f t="array" ref="M83">SUM($F$2:$F$79*(M$2:M$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>156</v>
-      </c>
-      <c r="N83" s="68">
-        <f t="array" ref="N83">SUM($F$2:$F$79*(N$2:N$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
+      <c r="M83" s="65">
+        <f t="array" ref="M83">SUM($F2:$F81*(M2:M81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
+        <v>138</v>
+      </c>
+      <c r="N83" s="65">
+        <f t="array" ref="N83">SUM($F2:$F81*(N2:N81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
         <v>146</v>
       </c>
-      <c r="O83" s="68">
-        <f t="array" ref="O83">SUM($F$2:$F$79*(O$2:O$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>156</v>
-      </c>
-      <c r="P83" s="68">
-        <f t="array" ref="P83">SUM($F$2:$F$79*(P$2:P$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>154</v>
-      </c>
-      <c r="Q83" s="69">
-        <f t="array" ref="Q83">SUM($F$2:$F$79*(Q$2:Q$79&gt;=0.1)*($V$2:$V$79&gt;=$X$12))</f>
-        <v>162</v>
+      <c r="O83" s="65">
+        <f t="array" ref="O83">SUM($F2:$F81*(O2:O81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
+        <v>140</v>
+      </c>
+      <c r="P83" s="65">
+        <f t="array" ref="P83">SUM($F2:$F81*(P2:P81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
+        <v>146</v>
+      </c>
+      <c r="Q83" s="66">
+        <f t="array" ref="Q83">SUM($F2:$F81*(Q2:Q81&gt;=0.9)*($V2:$V81&gt;=$X$12))</f>
+        <v>136</v>
       </c>
       <c r="R83" s="68"/>
       <c r="S83" s="68"/>
       <c r="T83" s="68"/>
       <c r="U83" s="68"/>
+      <c r="Y83" s="33"/>
+      <c r="Z83" s="33"/>
+      <c r="AA83" s="33"/>
+      <c r="AB83" s="6"/>
+      <c r="AC83" s="6"/>
+      <c r="AD83" s="6"/>
+      <c r="AE83" s="6"/>
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K84" s="67" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L84" s="68">
-        <f t="shared" ref="L84:Q84" si="5">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
-        <v>186</v>
+        <f t="array" ref="L84">SUM($F2:$F81*L2:L81*($V2:$V81&gt;=$X$12))</f>
+        <v>108</v>
       </c>
       <c r="M84" s="68">
-        <f t="shared" si="5"/>
-        <v>186</v>
+        <f t="array" ref="M84">SUM($F2:$F81*M2:M81*($V2:$V81&gt;=$X$12))</f>
+        <v>145.4</v>
       </c>
       <c r="N84" s="68">
-        <f t="shared" si="5"/>
-        <v>186</v>
+        <f t="array" ref="N84">SUM($F2:$F81*N2:N81*($V2:$V81&gt;=$X$12))</f>
+        <v>147</v>
       </c>
       <c r="O84" s="68">
-        <f t="shared" si="5"/>
-        <v>186</v>
+        <f t="array" ref="O84">SUM($F2:$F81*O2:O81*($V2:$V81&gt;=$X$12))</f>
+        <v>153.19999999999999</v>
       </c>
       <c r="P84" s="68">
-        <f t="shared" si="5"/>
-        <v>186</v>
+        <f t="array" ref="P84">SUM($F2:$F81*P2:P81*($V2:$V81&gt;=$X$12))</f>
+        <v>151.80000000000001</v>
       </c>
       <c r="Q84" s="69">
-        <f t="shared" si="5"/>
-        <v>186</v>
+        <f t="array" ref="Q84">SUM($F2:$F81*Q2:Q81*($V2:$V81&gt;=$X$12))</f>
+        <v>149</v>
       </c>
       <c r="R84" s="68"/>
       <c r="S84" s="68"/>
       <c r="T84" s="68"/>
       <c r="U84" s="68"/>
+      <c r="AB84" s="6"/>
+      <c r="AC84" s="6"/>
+      <c r="AD84" s="6"/>
+      <c r="AE84" s="6"/>
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.3">
       <c r="K85" s="67" t="s">
-        <v>169</v>
-      </c>
-      <c r="L85" s="70">
-        <f t="shared" ref="L85:N85" si="6">L82/L84</f>
-        <v>0.56989247311827962</v>
-      </c>
-      <c r="M85" s="70">
-        <f t="shared" si="6"/>
-        <v>0.7709677419354839</v>
-      </c>
-      <c r="N85" s="70">
-        <f t="shared" si="6"/>
-        <v>0.77956989247311825</v>
-      </c>
-      <c r="O85" s="70">
-        <f t="shared" ref="O85:P85" si="7">O82/O84</f>
-        <v>0.81505376344086022</v>
-      </c>
-      <c r="P85" s="70">
-        <f t="shared" si="7"/>
-        <v>0.80537634408602155</v>
-      </c>
-      <c r="Q85" s="71">
-        <f t="shared" ref="Q85" si="8">Q82/Q84</f>
-        <v>0.79032258064516125</v>
-      </c>
-      <c r="R85" s="70"/>
-      <c r="S85" s="70"/>
-      <c r="T85" s="70"/>
-      <c r="U85" s="70"/>
-    </row>
-    <row r="86" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D86" s="33"/>
-      <c r="K86" s="72" t="s">
-        <v>90</v>
-      </c>
-      <c r="L86" s="73">
-        <f t="array" ref="L86">SUM($F2:$F79*L2:L79*($V2:$V79&lt;$X$12))</f>
-        <v>10</v>
-      </c>
-      <c r="M86" s="73">
-        <f t="array" ref="M86">SUM($F2:$F79*M2:M79*($V2:$V79&lt;$X$12))</f>
-        <v>31.6</v>
-      </c>
-      <c r="N86" s="73">
-        <f t="array" ref="N86">SUM($F2:$F79*N2:N79*($V2:$V79&lt;$X$12))</f>
-        <v>32</v>
-      </c>
-      <c r="O86" s="73">
-        <f t="array" ref="O86">SUM($F2:$F79*O2:O79*($V2:$V79&lt;$X$12))</f>
-        <v>17.8</v>
-      </c>
-      <c r="P86" s="73">
-        <f t="array" ref="P86">SUM($F2:$F79*P2:P79*($V2:$V79&lt;$X$12))</f>
-        <v>19</v>
-      </c>
-      <c r="Q86" s="74">
-        <f t="array" ref="Q86">SUM($F2:$F79*Q2:Q79*($V2:$V79&lt;$X$12))</f>
-        <v>19.3</v>
+        <v>165</v>
+      </c>
+      <c r="L85" s="68">
+        <f t="array" ref="L85">SUM($F$2:$F$81*(L$2:L$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>110</v>
+      </c>
+      <c r="M85" s="68">
+        <f t="array" ref="M85">SUM($F$2:$F$81*(M$2:M$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>158</v>
+      </c>
+      <c r="N85" s="68">
+        <f t="array" ref="N85">SUM($F$2:$F$81*(N$2:N$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>148</v>
+      </c>
+      <c r="O85" s="68">
+        <f t="array" ref="O85">SUM($F$2:$F$81*(O$2:O$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>158</v>
+      </c>
+      <c r="P85" s="68">
+        <f t="array" ref="P85">SUM($F$2:$F$81*(P$2:P$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>156</v>
+      </c>
+      <c r="Q85" s="69">
+        <f t="array" ref="Q85">SUM($F$2:$F$81*(Q$2:Q$81&gt;=0.1)*($V$2:$V$81&gt;=$X$12))</f>
+        <v>164</v>
+      </c>
+      <c r="R85" s="68"/>
+      <c r="S85" s="68"/>
+      <c r="T85" s="68"/>
+      <c r="U85" s="68"/>
+    </row>
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="K86" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="L86" s="68">
+        <f t="shared" ref="L86:Q86" si="5">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
+        <v>188</v>
+      </c>
+      <c r="M86" s="68">
+        <f t="shared" si="5"/>
+        <v>188</v>
+      </c>
+      <c r="N86" s="68">
+        <f t="shared" si="5"/>
+        <v>188</v>
+      </c>
+      <c r="O86" s="68">
+        <f t="shared" si="5"/>
+        <v>188</v>
+      </c>
+      <c r="P86" s="68">
+        <f t="shared" si="5"/>
+        <v>188</v>
+      </c>
+      <c r="Q86" s="69">
+        <f t="shared" si="5"/>
+        <v>188</v>
       </c>
       <c r="R86" s="68"/>
       <c r="S86" s="68"/>
       <c r="T86" s="68"/>
       <c r="U86" s="68"/>
-      <c r="AA86" s="33"/>
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="D87" s="33"/>
-    </row>
-    <row r="88" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="K87" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="L87" s="70">
+        <f t="shared" ref="L87:N87" si="6">L84/L86</f>
+        <v>0.57446808510638303</v>
+      </c>
+      <c r="M87" s="70">
+        <f t="shared" si="6"/>
+        <v>0.77340425531914891</v>
+      </c>
+      <c r="N87" s="70">
+        <f t="shared" si="6"/>
+        <v>0.78191489361702127</v>
+      </c>
+      <c r="O87" s="70">
+        <f t="shared" ref="O87:P87" si="7">O84/O86</f>
+        <v>0.8148936170212765</v>
+      </c>
+      <c r="P87" s="70">
+        <f t="shared" si="7"/>
+        <v>0.80744680851063833</v>
+      </c>
+      <c r="Q87" s="71">
+        <f t="shared" ref="Q87" si="8">Q84/Q86</f>
+        <v>0.79255319148936165</v>
+      </c>
+      <c r="R87" s="70"/>
+      <c r="S87" s="70"/>
+      <c r="T87" s="70"/>
+      <c r="U87" s="70"/>
+    </row>
+    <row r="88" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D88" s="33"/>
-    </row>
-    <row r="89" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="10"/>
-      <c r="B89" s="23"/>
-      <c r="C89" s="23"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="14"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="20"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="20"/>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="34"/>
-      <c r="Q89" s="83"/>
-      <c r="R89" s="83"/>
-      <c r="S89" s="83"/>
-      <c r="T89" s="83"/>
-      <c r="U89" s="83"/>
-      <c r="V89" s="3"/>
-      <c r="W89" s="3"/>
-      <c r="X89" s="3"/>
-      <c r="Y89"/>
-      <c r="Z89"/>
-      <c r="AA89"/>
-      <c r="AB89"/>
-      <c r="AC89"/>
-      <c r="AD89"/>
-      <c r="AE89"/>
-    </row>
-    <row r="95" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="AB95" s="6"/>
-      <c r="AC95" s="6"/>
-      <c r="AD95" s="6"/>
-      <c r="AE95" s="6"/>
-    </row>
-    <row r="99" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB99" s="6"/>
-      <c r="AC99" s="6"/>
-      <c r="AD99" s="6"/>
-      <c r="AE99" s="6"/>
-    </row>
-    <row r="104" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB104" s="6"/>
-      <c r="AC104" s="6"/>
-      <c r="AD104" s="6"/>
-      <c r="AE104" s="6"/>
-    </row>
-    <row r="117" spans="28:31" x14ac:dyDescent="0.3">
-      <c r="AB117" s="33"/>
-      <c r="AC117" s="33"/>
-      <c r="AD117" s="33"/>
-      <c r="AE117" s="33"/>
+      <c r="K88" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="L88" s="73">
+        <f t="array" ref="L88">SUM($F2:$F81*L2:L81*($V2:$V81&lt;$X$12))</f>
+        <v>10</v>
+      </c>
+      <c r="M88" s="73">
+        <f t="array" ref="M88">SUM($F2:$F81*M2:M81*($V2:$V81&lt;$X$12))</f>
+        <v>31.6</v>
+      </c>
+      <c r="N88" s="73">
+        <f t="array" ref="N88">SUM($F2:$F81*N2:N81*($V2:$V81&lt;$X$12))</f>
+        <v>32</v>
+      </c>
+      <c r="O88" s="73">
+        <f t="array" ref="O88">SUM($F2:$F81*O2:O81*($V2:$V81&lt;$X$12))</f>
+        <v>17.8</v>
+      </c>
+      <c r="P88" s="73">
+        <f t="array" ref="P88">SUM($F2:$F81*P2:P81*($V2:$V81&lt;$X$12))</f>
+        <v>19</v>
+      </c>
+      <c r="Q88" s="74">
+        <f t="array" ref="Q88">SUM($F2:$F81*Q2:Q81*($V2:$V81&lt;$X$12))</f>
+        <v>19.3</v>
+      </c>
+      <c r="R88" s="68"/>
+      <c r="S88" s="68"/>
+      <c r="T88" s="68"/>
+      <c r="U88" s="68"/>
+      <c r="AA88" s="33"/>
+    </row>
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="D89" s="33"/>
+    </row>
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="D90" s="33"/>
+    </row>
+    <row r="91" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="10"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="20"/>
+      <c r="L91" s="2"/>
+      <c r="M91" s="20"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+      <c r="P91" s="34"/>
+      <c r="Q91" s="83"/>
+      <c r="R91" s="83"/>
+      <c r="S91" s="83"/>
+      <c r="T91" s="83"/>
+      <c r="U91" s="83"/>
+      <c r="V91" s="3"/>
+      <c r="W91" s="3"/>
+      <c r="X91" s="3"/>
+      <c r="Y91"/>
+      <c r="Z91"/>
+      <c r="AA91"/>
+      <c r="AB91"/>
+      <c r="AC91"/>
+      <c r="AD91"/>
+      <c r="AE91"/>
+    </row>
+    <row r="97" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB97" s="6"/>
+      <c r="AC97" s="6"/>
+      <c r="AD97" s="6"/>
+      <c r="AE97" s="6"/>
+    </row>
+    <row r="101" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB101" s="6"/>
+      <c r="AC101" s="6"/>
+      <c r="AD101" s="6"/>
+      <c r="AE101" s="6"/>
+    </row>
+    <row r="106" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB106" s="6"/>
+      <c r="AC106" s="6"/>
+      <c r="AD106" s="6"/>
+      <c r="AE106" s="6"/>
+    </row>
+    <row r="119" spans="28:31" x14ac:dyDescent="0.3">
+      <c r="AB119" s="33"/>
+      <c r="AC119" s="33"/>
+      <c r="AD119" s="33"/>
+      <c r="AE119" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:V79">
+  <conditionalFormatting sqref="B2:V81">
     <cfRule type="expression" dxfId="2" priority="40" stopIfTrue="1">
       <formula>$V2&gt;=(0.5+$X$12)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changes to Matt's version of the diffraction lab.  (Jerry's version unchanged.)
I incorporated a Mathematica simulation into the lab.  I also made slight changes to the activity numbering, making it easier to skip parts of the lab, for instructors who want to do different things.  Also added several color pictures, at Jerry's suggestion (good idea!).
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -2842,7 +2842,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4413,16 +4413,16 @@
         <v>0</v>
       </c>
       <c r="Y26" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X26,F$2:F$82)</f>
+        <f t="shared" ref="Y26:Y34" si="2">SUMIF(V$2:V$82,"&gt;=" &amp; X26,F$2:F$82)</f>
         <v>354</v>
       </c>
       <c r="Z26" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X26,E$2:E$82)</f>
-        <v>24</v>
+        <f t="shared" ref="Z26:Z34" si="3">SUMIF(V$2:V$82,"&gt;=" &amp; X26,E$2:E$82)</f>
+        <v>27</v>
       </c>
       <c r="AA26" s="8">
-        <f t="shared" ref="AA26:AA34" si="2">($Z$17 + $Z$15*Y26+$Z$16*Z26)*(1+Z$18+Z$19)</f>
-        <v>36.269999999999996</v>
+        <f t="shared" ref="AA26:AA34" si="4">($Z$17 + $Z$15*Y26+$Z$16*Z26)*(1+Z$18+Z$19)</f>
+        <v>37.44</v>
       </c>
       <c r="AB26" s="33"/>
       <c r="AC26" s="33"/>
@@ -4488,16 +4488,16 @@
         <v>0.5</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X27,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>286</v>
       </c>
       <c r="Z27" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X27,E$2:E$82)</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
       <c r="AA27" s="8">
-        <f t="shared" si="2"/>
-        <v>28.340000000000003</v>
+        <f t="shared" si="4"/>
+        <v>29.51</v>
       </c>
       <c r="AB27" s="33"/>
       <c r="AC27" s="33"/>
@@ -4571,16 +4571,16 @@
         <v>1</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X28,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>254</v>
       </c>
       <c r="Z28" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X28,E$2:E$82)</f>
-        <v>15</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
       <c r="AA28" s="8">
-        <f t="shared" si="2"/>
-        <v>26.260000000000005</v>
+        <f t="shared" si="4"/>
+        <v>27.430000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
@@ -4625,16 +4625,16 @@
         <v>1.5</v>
       </c>
       <c r="Y29" s="31">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X29,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>188</v>
       </c>
       <c r="Z29" s="31">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X29,E$2:E$82)</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="AA29" s="8">
-        <f t="shared" si="2"/>
-        <v>20.02</v>
+        <f t="shared" si="4"/>
+        <v>21.19</v>
       </c>
       <c r="AB29" s="33"/>
       <c r="AC29" s="33"/>
@@ -4680,16 +4680,16 @@
         <v>2</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X30,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="Z30" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X30,E$2:E$82)</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>13</v>
       </c>
       <c r="AA30" s="8">
-        <f t="shared" si="2"/>
-        <v>19.110000000000003</v>
+        <f t="shared" si="4"/>
+        <v>20.28</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
@@ -4748,16 +4748,16 @@
         <v>2.5</v>
       </c>
       <c r="Y31" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X31,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="Z31" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X31,E$2:E$82)</f>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AA31" s="8">
-        <f t="shared" si="2"/>
-        <v>14.170000000000002</v>
+        <f t="shared" si="4"/>
+        <v>15.340000000000002</v>
       </c>
       <c r="AB31" s="33"/>
       <c r="AC31" s="33"/>
@@ -4835,16 +4835,16 @@
         <v>3</v>
       </c>
       <c r="Y32" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X32,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>102</v>
       </c>
       <c r="Z32" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X32,E$2:E$82)</f>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="AA32" s="8">
-        <f t="shared" si="2"/>
-        <v>12.480000000000002</v>
+        <f t="shared" si="4"/>
+        <v>13.650000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:31" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4909,16 +4909,16 @@
         <v>3.5</v>
       </c>
       <c r="Y33" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X33,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="Z33" s="6">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X33,E$2:E$82)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="AA33" s="8">
-        <f t="shared" si="2"/>
-        <v>7.02</v>
+        <f t="shared" si="4"/>
+        <v>8.19</v>
       </c>
       <c r="AB33"/>
       <c r="AC33"/>
@@ -4996,16 +4996,16 @@
         <v>4</v>
       </c>
       <c r="Y34" s="47">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X34,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="Z34" s="47">
-        <f>SUMIF(V$2:V$82,"&gt;=" &amp; X34,E$2:E$82)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="AA34" s="9">
-        <f t="shared" si="2"/>
-        <v>6.63</v>
+        <f t="shared" si="4"/>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="35" spans="1:31" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -5729,10 +5729,10 @@
         <v>209</v>
       </c>
       <c r="D47" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E47" s="14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F47" s="14">
         <f t="shared" si="0"/>
@@ -7162,7 +7162,7 @@
       </c>
       <c r="U73" s="84"/>
       <c r="V73" s="75">
-        <f t="shared" ref="V73:V81" si="3">SUM(R73:U73)</f>
+        <f t="shared" ref="V73:V81" si="5">SUM(R73:U73)</f>
         <v>2</v>
       </c>
       <c r="X73" s="3"/>
@@ -7187,7 +7187,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="14">
-        <f t="shared" ref="F74:F81" si="4">CEILING(D74,X$22+1)</f>
+        <f t="shared" ref="F74:F81" si="6">CEILING(D74,X$22+1)</f>
         <v>2</v>
       </c>
       <c r="K74" s="22" t="s">
@@ -7213,7 +7213,7 @@
       </c>
       <c r="U74" s="85"/>
       <c r="V74" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W74" s="33"/>
@@ -7231,7 +7231,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G75" s="14"/>
@@ -7265,7 +7265,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K76" s="22"/>
@@ -7297,7 +7297,7 @@
         <v>1</v>
       </c>
       <c r="V76" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="W76" s="33"/>
@@ -7318,7 +7318,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G77" s="14"/>
@@ -7353,7 +7353,7 @@
       </c>
       <c r="U77" s="83"/>
       <c r="V77" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W77" s="15"/>
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K78" s="22"/>
@@ -7390,7 +7390,7 @@
       <c r="T78" s="33"/>
       <c r="U78" s="33"/>
       <c r="V78" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W78" s="15"/>
@@ -7406,7 +7406,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K79" s="22"/>
@@ -7419,7 +7419,7 @@
       <c r="T79" s="33"/>
       <c r="U79" s="33"/>
       <c r="V79" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W79" s="15"/>
@@ -7439,7 +7439,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K80" s="22"/>
@@ -7454,7 +7454,7 @@
       <c r="T80" s="33"/>
       <c r="U80" s="33"/>
       <c r="V80" s="75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W80" s="15"/>
@@ -7472,7 +7472,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G81" s="27"/>
@@ -7505,7 +7505,7 @@
       </c>
       <c r="U81" s="86"/>
       <c r="V81" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="W81" s="15"/>
@@ -7636,27 +7636,27 @@
         <v>167</v>
       </c>
       <c r="L86" s="68">
-        <f t="shared" ref="L86:Q86" si="5">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
+        <f t="shared" ref="L86:Q86" si="7">LOOKUP($X$12,$X26:$X34,$Y26:$Y34)</f>
         <v>188</v>
       </c>
       <c r="M86" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="N86" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="O86" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="P86" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="Q86" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>188</v>
       </c>
       <c r="R86" s="68"/>
@@ -7669,27 +7669,27 @@
         <v>168</v>
       </c>
       <c r="L87" s="70">
-        <f t="shared" ref="L87:N87" si="6">L84/L86</f>
+        <f t="shared" ref="L87:N87" si="8">L84/L86</f>
         <v>0.57446808510638303</v>
       </c>
       <c r="M87" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.77340425531914891</v>
       </c>
       <c r="N87" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.78191489361702127</v>
       </c>
       <c r="O87" s="70">
-        <f t="shared" ref="O87:P87" si="7">O84/O86</f>
+        <f t="shared" ref="O87:P87" si="9">O84/O86</f>
         <v>0.8148936170212765</v>
       </c>
       <c r="P87" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.80744680851063833</v>
       </c>
       <c r="Q87" s="71">
-        <f t="shared" ref="Q87" si="8">Q84/Q86</f>
+        <f t="shared" ref="Q87" si="10">Q84/Q86</f>
         <v>0.79255319148936165</v>
       </c>
       <c r="R87" s="70"/>

</xml_diff>

<commit_message>
Updated color page index entries
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -2894,9 +2894,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U89" sqref="U89"/>
+      <selection pane="bottomLeft" activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3005,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="54">
-        <f>CEILING(D2,W$22+1)</f>
+        <f t="shared" ref="F2:F33" si="0">CEILING(D2,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G2" s="54"/>
@@ -3051,7 +3051,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="58">
-        <f>CEILING(D3,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G3" s="58"/>
@@ -3071,7 +3071,7 @@
         <v>2</v>
       </c>
       <c r="U3" s="81">
-        <f t="shared" ref="U3:U66" si="0">SUM(Q3:T3)</f>
+        <f t="shared" ref="U3:U66" si="1">SUM(Q3:T3)</f>
         <v>2</v>
       </c>
       <c r="V3" s="31"/>
@@ -3101,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <f>CEILING(D4,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G4" s="13">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="T4" s="77"/>
       <c r="U4" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V4" s="31"/>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="13">
-        <f>CEILING(D5,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G5" s="13">
@@ -3208,7 +3208,7 @@
         <v>1</v>
       </c>
       <c r="U5" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V5" s="31"/>
@@ -3236,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="13">
-        <f>CEILING(D6,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H6" s="13">
@@ -3264,7 +3264,7 @@
       </c>
       <c r="T6" s="77"/>
       <c r="U6" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V6" s="31"/>
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="26">
-        <f>CEILING(D7,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G7" s="26"/>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="T7" s="78"/>
       <c r="U7" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W7" s="5"/>
@@ -3339,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="13">
-        <f>CEILING(D8,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I8" s="13">
@@ -3373,7 +3373,7 @@
         <v>0.5</v>
       </c>
       <c r="U8" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="V8" s="31"/>
@@ -3400,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="13">
-        <f>CEILING(D9,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H9" s="13">
@@ -3434,7 +3434,7 @@
         <v>1</v>
       </c>
       <c r="U9" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V9" s="31"/>
@@ -3461,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="13">
-        <f>CEILING(D10,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G10" s="13">
@@ -3483,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="U10" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V10" s="31"/>
@@ -3510,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="13">
-        <f>CEILING(D11,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11" s="13">
@@ -3544,7 +3544,7 @@
         <v>1</v>
       </c>
       <c r="U11" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V11" s="31"/>
@@ -3573,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="13">
-        <f>CEILING(D12,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K12" s="21" t="s">
@@ -3594,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="U12" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V12" s="31"/>
@@ -3623,7 +3623,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="13">
-        <f>CEILING(D13,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K13" s="21" t="s">
@@ -3644,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="U13" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="V13" s="31"/>
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="13">
-        <f>CEILING(D14,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K14" s="21"/>
@@ -3679,7 +3679,7 @@
       <c r="M14" s="75"/>
       <c r="S14" s="77"/>
       <c r="U14" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V14" s="31"/>
@@ -3707,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="13">
-        <f>CEILING(D15,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K15" s="21"/>
@@ -3715,7 +3715,7 @@
       <c r="M15" s="75"/>
       <c r="S15" s="77"/>
       <c r="U15" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V15" s="31"/>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="13">
-        <f>CEILING(D16,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="K16" s="21" t="s">
@@ -3774,7 +3774,7 @@
         <v>1</v>
       </c>
       <c r="U16" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V16" s="31"/>
@@ -3805,7 +3805,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="13">
-        <f>CEILING(D17,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G17" s="13">
@@ -3846,7 +3846,7 @@
         <v>1</v>
       </c>
       <c r="U17" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V17" s="31"/>
@@ -3877,7 +3877,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="13">
-        <f>CEILING(D18,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K18" s="21" t="s">
@@ -3936,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="13">
-        <f>CEILING(D19,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K19" s="21" t="s">
@@ -3964,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="U19" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="V19" s="31"/>
@@ -3995,7 +3995,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="13">
-        <f>CEILING(D20,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H20" s="13">
@@ -4032,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="U20" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="V20" s="31"/>
@@ -4056,7 +4056,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="13">
-        <f>CEILING(D21,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G21" s="13">
@@ -4067,7 +4067,7 @@
       <c r="M21" s="31"/>
       <c r="S21" s="77"/>
       <c r="U21" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V21" s="31"/>
@@ -4096,7 +4096,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="13">
-        <f>CEILING(D22,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G22" s="13">
@@ -4111,7 +4111,7 @@
         <v>0.4</v>
       </c>
       <c r="U22" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="V22" s="31"/>
@@ -4140,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="13">
-        <f>CEILING(D23,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G23" s="13">
@@ -4168,7 +4168,7 @@
       </c>
       <c r="T23" s="78"/>
       <c r="U23" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V23" s="31"/>
@@ -4197,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="12">
-        <f>CEILING(D24,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="G24" s="12"/>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="T24" s="77"/>
       <c r="U24" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V24" s="31"/>
@@ -4260,7 +4260,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="13">
-        <f>CEILING(D25,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H25" s="13">
@@ -4300,7 +4300,7 @@
         <v>1</v>
       </c>
       <c r="U25" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V25" s="31"/>
@@ -4335,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="13">
-        <f>CEILING(D26,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K26" s="21"/>
@@ -4350,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="U26" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V26" s="31"/>
@@ -4358,15 +4358,15 @@
         <v>0</v>
       </c>
       <c r="X26" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,F$2:F$82)</f>
+        <f t="shared" ref="X26:X34" si="2">SUMIF(U$2:U$82,"&gt;=" &amp; W26,F$2:F$82)</f>
         <v>356</v>
       </c>
       <c r="Y26" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W26,E$2:E$82)</f>
+        <f t="shared" ref="Y26:Y34" si="3">SUMIF(U$2:U$82,"&gt;=" &amp; W26,E$2:E$82)</f>
         <v>28</v>
       </c>
       <c r="Z26" s="8">
-        <f t="shared" ref="Z26:Z34" si="1">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
+        <f t="shared" ref="Z26:Z34" si="4">($Y$17 + $Y$15*X26+$Y$16*Y26)*(1+Y$18+Y$19)</f>
         <v>37.960000000000008</v>
       </c>
       <c r="AA26" s="31"/>
@@ -4388,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="13">
-        <f>CEILING(D27,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H27" s="13">
@@ -4419,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="U27" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V27" s="31"/>
@@ -4427,15 +4427,15 @@
         <v>0.5</v>
       </c>
       <c r="X27" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>272</v>
       </c>
       <c r="Y27" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W27,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="Z27" s="8">
-        <f t="shared" si="1"/>
+        <f>($Y$17 + $Y$15*X27+$Y$16*Y27)*(1+Y$18+Y$19)</f>
         <v>28.6</v>
       </c>
       <c r="AA27" s="31"/>
@@ -4458,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="F28" s="13">
-        <f>CEILING(D28,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G28" s="13"/>
@@ -4498,22 +4498,22 @@
       </c>
       <c r="T28" s="75"/>
       <c r="U28" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="W28" s="69">
         <v>1</v>
       </c>
       <c r="X28" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>262</v>
       </c>
       <c r="Y28" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W28,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="Z28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>27.95</v>
       </c>
     </row>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="13">
-        <f>CEILING(D29,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G29" s="13">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="S29" s="77"/>
       <c r="U29" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V29" s="31"/>
@@ -4557,15 +4557,15 @@
         <v>1.5</v>
       </c>
       <c r="X29" s="29">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>142</v>
       </c>
       <c r="Y29" s="29">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W29,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="Z29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17.420000000000002</v>
       </c>
       <c r="AA29" s="31"/>
@@ -4587,7 +4587,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="13">
-        <f>CEILING(D30,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K30" s="55" t="s">
@@ -4603,7 +4603,7 @@
       <c r="S30" s="77"/>
       <c r="T30" s="78"/>
       <c r="U30" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V30" s="31"/>
@@ -4611,15 +4611,15 @@
         <v>2</v>
       </c>
       <c r="X30" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="Y30" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W30,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="Z30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>16.64</v>
       </c>
     </row>
@@ -4640,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="12">
-        <f>CEILING(D31,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G31" s="12">
@@ -4666,7 +4666,7 @@
       <c r="S31" s="76"/>
       <c r="T31" s="77"/>
       <c r="U31" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V31" s="31"/>
@@ -4674,15 +4674,15 @@
         <v>2.5</v>
       </c>
       <c r="X31" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>66</v>
       </c>
       <c r="Y31" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W31,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="Z31" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10.530000000000003</v>
       </c>
       <c r="AA31" s="31"/>
@@ -4704,7 +4704,7 @@
         <v>0</v>
       </c>
       <c r="F32" s="13">
-        <f>CEILING(D32,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G32" s="13">
@@ -4747,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="U32" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V32" s="31"/>
@@ -4755,15 +4755,15 @@
         <v>3</v>
       </c>
       <c r="X32" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W32,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="Y32" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W32,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="Z32" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8.1900000000000013</v>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="13">
-        <f>CEILING(D33,W$22+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G33" s="13"/>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="T33" s="75"/>
       <c r="U33" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V33" s="31"/>
@@ -4826,15 +4826,15 @@
         <v>3.5</v>
       </c>
       <c r="X33" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W33,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Y33" s="6">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W33,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z33" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.8099999999999996</v>
       </c>
       <c r="AA33"/>
@@ -4856,7 +4856,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="13">
-        <f>CEILING(D34,W$22+1)</f>
+        <f t="shared" ref="F34:F65" si="5">CEILING(D34,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G34" s="13">
@@ -4899,7 +4899,7 @@
         <v>1</v>
       </c>
       <c r="U34" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V34" s="31"/>
@@ -4907,15 +4907,15 @@
         <v>4</v>
       </c>
       <c r="X34" s="45">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W34,F$2:F$82)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Y34" s="45">
-        <f>SUMIF(U$2:U$82,"&gt;=" &amp; W34,E$2:E$82)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="Z34" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.8099999999999996</v>
       </c>
     </row>
@@ -4934,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="F35" s="13">
-        <f>CEILING(D35,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G35" s="13">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="T35" s="75"/>
       <c r="U35" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="W35" s="3"/>
@@ -4990,7 +4990,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="13">
-        <f>CEILING(D36,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H36" s="13">
@@ -5021,7 +5021,7 @@
         <v>1</v>
       </c>
       <c r="U36" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V36" s="31"/>
@@ -5044,7 +5044,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="13">
-        <f>CEILING(D37,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J37" s="13">
@@ -5069,7 +5069,7 @@
         <v>1</v>
       </c>
       <c r="U37" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V37" s="31"/>
@@ -5091,7 +5091,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="13">
-        <f>CEILING(D38,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J38" s="13">
@@ -5119,7 +5119,7 @@
         <v>1</v>
       </c>
       <c r="U38" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V38" s="31"/>
@@ -5142,7 +5142,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="13">
-        <f>CEILING(D39,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G39" s="13">
@@ -5184,7 +5184,7 @@
       </c>
       <c r="T39" s="78"/>
       <c r="U39" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V39" s="31"/>
@@ -5207,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="12">
-        <f>CEILING(D40,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G40" s="12" t="s">
@@ -5251,7 +5251,7 @@
       </c>
       <c r="T40" s="77"/>
       <c r="U40" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V40" s="31"/>
@@ -5271,7 +5271,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="13">
-        <f>CEILING(D41,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G41" s="13">
@@ -5309,7 +5309,7 @@
         <v>1</v>
       </c>
       <c r="U41" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V41" s="31"/>
@@ -5331,7 +5331,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="13">
-        <f>CEILING(D42,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G42" s="13"/>
@@ -5351,7 +5351,7 @@
       <c r="S42" s="77"/>
       <c r="T42" s="75"/>
       <c r="U42" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V42" s="31"/>
@@ -5378,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="13">
-        <f>CEILING(D43,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H43" s="13">
@@ -5410,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="U43" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V43" s="31"/>
@@ -5431,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="F44" s="13">
-        <f>CEILING(D44,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G44" s="13" t="s">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V44" s="31"/>
@@ -5489,7 +5489,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="12">
-        <f>CEILING(D45,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G45" s="12" t="s">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="T45" s="77"/>
       <c r="U45" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V45" s="31"/>
@@ -5553,7 +5553,7 @@
         <v>2</v>
       </c>
       <c r="F46" s="13">
-        <f>CEILING(D46,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G46" s="13"/>
@@ -5573,7 +5573,7 @@
       <c r="S46" s="77"/>
       <c r="T46" s="77"/>
       <c r="U46" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W46" s="3"/>
@@ -5592,7 +5592,7 @@
         <v>3</v>
       </c>
       <c r="F47" s="13">
-        <f>CEILING(D47,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G47" s="13" t="s">
@@ -5635,7 +5635,7 @@
         <v>0.9</v>
       </c>
       <c r="U47" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
       <c r="V47" s="31"/>
@@ -5660,7 +5660,7 @@
         <v>4</v>
       </c>
       <c r="F48" s="13">
-        <f>CEILING(D48,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G48" s="13"/>
@@ -5680,7 +5680,7 @@
       <c r="S48" s="77"/>
       <c r="T48" s="75"/>
       <c r="U48" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W48" s="3"/>
@@ -5705,7 +5705,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="13">
-        <f>CEILING(D49,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G49" s="13">
@@ -5745,7 +5745,7 @@
       </c>
       <c r="T49" s="75"/>
       <c r="U49" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
       <c r="V49" s="31"/>
@@ -5771,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="13">
-        <f>CEILING(D50,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G50" s="13">
@@ -5797,7 +5797,7 @@
       <c r="S50" s="77"/>
       <c r="T50" s="78"/>
       <c r="U50" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V50" s="31"/>
@@ -5820,7 +5820,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="12">
-        <f>CEILING(D51,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G51" s="12">
@@ -5852,7 +5852,7 @@
       <c r="S51" s="76"/>
       <c r="T51" s="77"/>
       <c r="U51" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V51" s="31"/>
@@ -5872,7 +5872,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="13">
-        <f>CEILING(D52,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G52" s="13">
@@ -5904,7 +5904,7 @@
       <c r="S52" s="77"/>
       <c r="T52" s="78"/>
       <c r="U52" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V52" s="31"/>
@@ -5934,7 +5934,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="12">
-        <f>CEILING(D53,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G53" s="12"/>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="T53" s="77"/>
       <c r="U53" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V53" s="31"/>
@@ -5988,7 +5988,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="13">
-        <f>CEILING(D54,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G54" s="13">
@@ -6028,7 +6028,7 @@
       </c>
       <c r="T54" s="75"/>
       <c r="U54" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V54" s="31"/>
@@ -6053,7 +6053,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="13">
-        <f>CEILING(D55,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G55" s="13">
@@ -6082,7 +6082,7 @@
         <v>0</v>
       </c>
       <c r="U55" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V55" s="31"/>
@@ -6101,7 +6101,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="13">
-        <f>CEILING(D56,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G56" s="13">
@@ -6119,7 +6119,7 @@
         <v>0</v>
       </c>
       <c r="U56" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V56" s="31"/>
@@ -6142,7 +6142,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="13">
-        <f>CEILING(D57,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="G57" s="13">
@@ -6180,7 +6180,7 @@
         <v>0.2</v>
       </c>
       <c r="U57" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="V57" s="31"/>
@@ -6200,7 +6200,7 @@
         <v>1</v>
       </c>
       <c r="F58" s="13">
-        <f>CEILING(D58,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G58" s="13">
@@ -6238,7 +6238,7 @@
         <v>1</v>
       </c>
       <c r="U58" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="V58" s="31"/>
@@ -6258,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="13">
-        <f>CEILING(D59,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="G59" s="13">
@@ -6293,7 +6293,7 @@
         <v>0.2</v>
       </c>
       <c r="U59" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="V59" s="31"/>
@@ -6314,7 +6314,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="13">
-        <f>CEILING(D60,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="H60" s="13">
@@ -6351,7 +6351,7 @@
         <v>1</v>
       </c>
       <c r="U60" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="V60" s="31"/>
@@ -6371,7 +6371,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="13">
-        <f>CEILING(D61,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J61" s="13">
@@ -6391,7 +6391,7 @@
         <v>0.5</v>
       </c>
       <c r="U61" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="V61" s="31"/>
@@ -6412,7 +6412,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="13">
-        <f>CEILING(D62,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J62" s="13">
@@ -6434,7 +6434,7 @@
         <v>1</v>
       </c>
       <c r="U62" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V62" s="31"/>
@@ -6454,7 +6454,7 @@
         <v>2</v>
       </c>
       <c r="F63" s="13">
-        <f>CEILING(D63,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="G63" s="13">
@@ -6470,7 +6470,7 @@
         <v>0</v>
       </c>
       <c r="U63" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V63" s="31"/>
@@ -6490,7 +6490,7 @@
         <v>1</v>
       </c>
       <c r="F64" s="13">
-        <f>CEILING(D64,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G64" s="13">
@@ -6507,7 +6507,7 @@
       </c>
       <c r="S64" s="77"/>
       <c r="U64" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V64" s="31"/>
@@ -6530,7 +6530,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="13">
-        <f>CEILING(D65,W$22+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J65" s="13">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="T65" s="78"/>
       <c r="U65" s="81">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V65" s="31"/>
@@ -6575,7 +6575,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="12">
-        <f>CEILING(D66,W$22+1)</f>
+        <f t="shared" ref="F66:F81" si="6">CEILING(D66,W$22+1)</f>
         <v>4</v>
       </c>
       <c r="G66" s="12">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="T66" s="77"/>
       <c r="U66" s="67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="V66" s="31"/>
@@ -6630,7 +6630,7 @@
         <v>2</v>
       </c>
       <c r="F67" s="13">
-        <f>CEILING(D67,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G67" s="13">
@@ -6652,7 +6652,7 @@
       <c r="S67" s="77"/>
       <c r="T67" s="75"/>
       <c r="U67" s="67">
-        <f t="shared" ref="U67:U81" si="2">SUM(Q67:T67)</f>
+        <f t="shared" ref="U67:U81" si="7">SUM(Q67:T67)</f>
         <v>1</v>
       </c>
       <c r="V67" s="31"/>
@@ -6679,7 +6679,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="13">
-        <f>CEILING(D68,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G68" s="13">
@@ -6690,7 +6690,7 @@
       <c r="M68" s="31"/>
       <c r="S68" s="77"/>
       <c r="U68" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V68" s="31"/>
@@ -6710,7 +6710,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="26">
-        <f>CEILING(D69,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="G69" s="26">
@@ -6734,7 +6734,7 @@
       <c r="S69" s="78"/>
       <c r="T69" s="78"/>
       <c r="U69" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V69" s="31"/>
@@ -6756,7 +6756,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="13">
-        <f>CEILING(D70,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G70" s="13">
@@ -6769,7 +6769,7 @@
       <c r="M70" s="31"/>
       <c r="S70" s="77"/>
       <c r="U70" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V70" s="31"/>
@@ -6791,7 +6791,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="13">
-        <f>CEILING(D71,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G71" s="13">
@@ -6811,7 +6811,7 @@
       <c r="S71" s="77"/>
       <c r="T71" s="75"/>
       <c r="U71" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V71" s="31"/>
@@ -6838,7 +6838,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="13">
-        <f>CEILING(D72,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K72" s="21" t="s">
@@ -6849,7 +6849,7 @@
       <c r="S72" s="77"/>
       <c r="T72" s="78"/>
       <c r="U72" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V72" s="31"/>
@@ -6873,7 +6873,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="12">
-        <f>CEILING(D73,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G73" s="12"/>
@@ -6903,7 +6903,7 @@
       </c>
       <c r="T73" s="77"/>
       <c r="U73" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
       <c r="W73" s="3"/>
@@ -6928,7 +6928,7 @@
         <v>1</v>
       </c>
       <c r="F74" s="13">
-        <f>CEILING(D74,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K74" s="21" t="s">
@@ -6952,7 +6952,7 @@
       <c r="S74" s="77"/>
       <c r="T74" s="77"/>
       <c r="U74" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V74" s="31"/>
@@ -6970,7 +6970,7 @@
         <v>1</v>
       </c>
       <c r="F75" s="13">
-        <f>CEILING(D75,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G75" s="13"/>
@@ -6994,7 +6994,7 @@
         <v>2</v>
       </c>
       <c r="U75" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="W75" s="3"/>
@@ -7010,7 +7010,7 @@
         <v>3</v>
       </c>
       <c r="F76" s="13">
-        <f>CEILING(D76,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K76" s="21"/>
@@ -7033,7 +7033,7 @@
         <v>1</v>
       </c>
       <c r="U76" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V76" s="31"/>
@@ -7054,7 +7054,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="13">
-        <f>CEILING(D77,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G77" s="13"/>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="T77" s="75"/>
       <c r="U77" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="V77" s="14"/>
@@ -7110,7 +7110,7 @@
         <v>1</v>
       </c>
       <c r="F78" s="13">
-        <f>CEILING(D78,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K78" s="21"/>
@@ -7118,7 +7118,7 @@
       <c r="M78" s="75"/>
       <c r="S78" s="77"/>
       <c r="U78" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V78" s="14"/>
@@ -7134,7 +7134,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="13">
-        <f>CEILING(D79,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K79" s="21"/>
@@ -7142,7 +7142,7 @@
       <c r="M79" s="75"/>
       <c r="S79" s="77"/>
       <c r="U79" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V79" s="14"/>
@@ -7162,7 +7162,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="13">
-        <f>CEILING(D80,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K80" s="21"/>
@@ -7170,7 +7170,7 @@
       <c r="M80" s="75"/>
       <c r="S80" s="77"/>
       <c r="U80" s="67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="V80" s="14"/>
@@ -7188,7 +7188,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="26">
-        <f>CEILING(D81,W$22+1)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G81" s="26"/>
@@ -7218,7 +7218,7 @@
       </c>
       <c r="T81" s="78"/>
       <c r="U81" s="81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="V81" s="14"/>
@@ -7347,15 +7347,15 @@
         <v>166</v>
       </c>
       <c r="Q87" s="64">
-        <f t="shared" ref="Q87:S87" si="3">Q84/Q86</f>
+        <f t="shared" ref="Q87:S87" si="8">Q84/Q86</f>
         <v>0.41221374045801529</v>
       </c>
       <c r="R87" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.38931297709923662</v>
       </c>
       <c r="S87" s="64">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.46488549618320613</v>
       </c>
       <c r="T87" s="64"/>

</xml_diff>

<commit_message>
updated labs for spring 2020, still not final.
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -15,7 +15,7 @@
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -986,7 +986,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="237">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -1575,9 +1575,6 @@
     <t>Not updated for Capstone</t>
   </si>
   <si>
-    <t>Not updated for Tracker</t>
-  </si>
-  <si>
     <t>2018 spr Ovidiu</t>
   </si>
   <si>
@@ -1633,18 +1630,6 @@
   </si>
   <si>
     <t>2019 spr Mariama</t>
-  </si>
-  <si>
-    <t>13 The Electric Field and the Electric Potential I</t>
-  </si>
-  <si>
-    <t>14 The Electric Field and the Electric Potential II</t>
-  </si>
-  <si>
-    <t>15 The Electric Field and the Electric Potential III</t>
-  </si>
-  <si>
-    <t>16 The Electric Field and the Electric Potential IV</t>
   </si>
   <si>
     <t>Using Digital Multimeters</t>
@@ -1689,6 +1674,33 @@
   </si>
   <si>
     <t>by MT, updated 2019</t>
+  </si>
+  <si>
+    <t>Electric Charges, Fields and Potentials For a Point Charge</t>
+  </si>
+  <si>
+    <t>Electric Charges, Fields and Potentials For a Dipole</t>
+  </si>
+  <si>
+    <t>The Electric Field and the Electric Potential III</t>
+  </si>
+  <si>
+    <t>The Electric Field and the Electric Potential IV</t>
+  </si>
+  <si>
+    <t>uses pretty old software</t>
+  </si>
+  <si>
+    <t>pages in common</t>
+  </si>
+  <si>
+    <t>js &amp; gpg</t>
+  </si>
+  <si>
+    <t>js&amp;mt</t>
+  </si>
+  <si>
+    <t>gpg&amp;mt</t>
   </si>
 </sst>
 </file>
@@ -2561,7 +2573,49 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2894,9 +2948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2905,7 +2959,8 @@
     <col min="2" max="2" width="53.77734375" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" style="22" customWidth="1"/>
     <col min="4" max="4" width="8.109375" style="13" customWidth="1"/>
-    <col min="5" max="10" width="5.77734375" style="13" customWidth="1"/>
+    <col min="5" max="6" width="5.77734375" style="13" customWidth="1"/>
+    <col min="7" max="10" width="5.77734375" style="13" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="30.109375" style="19" customWidth="1"/>
     <col min="12" max="13" width="8.77734375" style="2" customWidth="1"/>
     <col min="14" max="20" width="8.77734375" style="75" customWidth="1"/>
@@ -2924,7 +2979,7 @@
         <v>107</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D1" s="48" t="s">
         <v>85</v>
@@ -2933,7 +2988,7 @@
         <v>86</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G1" s="48" t="s">
         <v>176</v>
@@ -2954,31 +3009,31 @@
         <v>100</v>
       </c>
       <c r="M1" s="47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N1" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="47" t="s">
         <v>213</v>
       </c>
-      <c r="O1" s="47" t="s">
-        <v>214</v>
-      </c>
       <c r="P1" s="47" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="Q1" s="47" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="R1" s="47" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="S1" s="47" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="T1" s="47" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="U1" s="50" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="V1" s="30"/>
       <c r="W1" s="31"/>
@@ -3018,15 +3073,21 @@
       <c r="N2" s="79"/>
       <c r="O2" s="79"/>
       <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="56"/>
+      <c r="Q2" s="79">
+        <v>1</v>
+      </c>
+      <c r="R2" s="79">
+        <v>1</v>
+      </c>
+      <c r="S2" s="56">
+        <v>1</v>
+      </c>
       <c r="T2" s="79">
         <v>2</v>
       </c>
       <c r="U2" s="67">
         <f>SUM(Q2:T2)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V2" s="31"/>
       <c r="W2" s="68"/>
@@ -3064,15 +3125,21 @@
       <c r="N3" s="80"/>
       <c r="O3" s="80"/>
       <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="57"/>
+      <c r="Q3" s="80">
+        <v>1</v>
+      </c>
+      <c r="R3" s="80">
+        <v>1</v>
+      </c>
+      <c r="S3" s="57">
+        <v>1</v>
+      </c>
       <c r="T3" s="80">
         <v>2</v>
       </c>
       <c r="U3" s="81">
         <f t="shared" ref="U3:U66" si="1">SUM(Q3:T3)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V3" s="31"/>
       <c r="W3" s="68"/>
@@ -3092,7 +3159,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" s="13">
         <v>5</v>
@@ -3161,7 +3228,7 @@
         <v>156</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" s="13">
         <v>2</v>
@@ -3227,7 +3294,7 @@
         <v>157</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" s="13">
         <v>2</v>
@@ -3283,7 +3350,7 @@
         <v>180</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="26">
         <v>1</v>
@@ -3330,7 +3397,7 @@
         <v>172</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" s="13">
         <v>4</v>
@@ -3370,11 +3437,11 @@
         <v>1</v>
       </c>
       <c r="S8" s="77">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="U8" s="67">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V8" s="31"/>
       <c r="W8" s="5"/>
@@ -3391,7 +3458,7 @@
         <v>111</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -3452,7 +3519,7 @@
         <v>112</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="13">
         <v>5</v>
@@ -3477,14 +3544,14 @@
       <c r="L10" s="32"/>
       <c r="M10" s="31"/>
       <c r="Q10" s="75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S10" s="77">
         <v>0</v>
       </c>
       <c r="U10" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="V10" s="31"/>
       <c r="W10" s="5"/>
@@ -3501,7 +3568,7 @@
         <v>113</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" s="13">
         <v>2</v>
@@ -3561,10 +3628,10 @@
     </row>
     <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="13">
         <v>4</v>
@@ -3577,7 +3644,7 @@
         <v>4</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L12" s="75"/>
       <c r="M12" s="75"/>
@@ -3599,7 +3666,7 @@
       </c>
       <c r="V12" s="31"/>
       <c r="W12" s="42">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="X12" s="43"/>
       <c r="Y12" s="5"/>
@@ -3611,10 +3678,10 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13" s="13">
         <v>3</v>
@@ -3627,7 +3694,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="L13" s="75"/>
       <c r="M13" s="75"/>
@@ -3659,10 +3726,10 @@
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D14" s="13">
         <v>3</v>
@@ -3674,7 +3741,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K14" s="21"/>
+      <c r="K14" s="21" t="s">
+        <v>232</v>
+      </c>
       <c r="L14" s="75"/>
       <c r="M14" s="75"/>
       <c r="S14" s="77"/>
@@ -3695,10 +3764,10 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="13">
         <v>3</v>
@@ -3710,7 +3779,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K15" s="21"/>
+      <c r="K15" s="21" t="s">
+        <v>232</v>
+      </c>
       <c r="L15" s="75"/>
       <c r="M15" s="75"/>
       <c r="S15" s="77"/>
@@ -3737,7 +3808,7 @@
         <v>182</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D16" s="13">
         <v>9</v>
@@ -3796,7 +3867,7 @@
         <v>185</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D17" s="13">
         <v>3</v>
@@ -3868,7 +3939,7 @@
         <v>183</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D18" s="13">
         <v>5</v>
@@ -3895,9 +3966,6 @@
       <c r="O18" s="75">
         <v>0.5</v>
       </c>
-      <c r="Q18" s="75">
-        <v>1</v>
-      </c>
       <c r="R18" s="75">
         <v>0.5</v>
       </c>
@@ -3905,8 +3973,8 @@
         <v>1</v>
       </c>
       <c r="U18" s="67">
-        <f>SUM(Q18:T18)</f>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>1.5</v>
       </c>
       <c r="V18" s="31"/>
       <c r="W18" s="17" t="s">
@@ -3927,7 +3995,7 @@
         <v>184</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D19" s="13">
         <v>4</v>
@@ -3957,6 +4025,9 @@
       <c r="P19" s="75">
         <v>1</v>
       </c>
+      <c r="Q19" s="75">
+        <v>1</v>
+      </c>
       <c r="R19" s="75">
         <v>0.5</v>
       </c>
@@ -3965,7 +4036,7 @@
       </c>
       <c r="U19" s="67">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="V19" s="31"/>
       <c r="W19" s="18" t="s">
@@ -3986,7 +4057,7 @@
         <v>114</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
@@ -4022,9 +4093,6 @@
       <c r="P20" s="75">
         <v>1</v>
       </c>
-      <c r="Q20" s="75">
-        <v>1</v>
-      </c>
       <c r="R20" s="75">
         <v>0.5</v>
       </c>
@@ -4033,7 +4101,7 @@
       </c>
       <c r="U20" s="67">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="V20" s="31"/>
       <c r="Z20" s="31"/>
@@ -4047,7 +4115,7 @@
         <v>115</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="13">
         <v>3</v>
@@ -4072,7 +4140,7 @@
       </c>
       <c r="V21" s="31"/>
       <c r="W21" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X21" s="41"/>
       <c r="Y21" s="31"/>
@@ -4087,7 +4155,7 @@
         <v>116</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="13">
         <v>4</v>
@@ -4108,11 +4176,11 @@
         <v>1</v>
       </c>
       <c r="S22" s="77">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="U22" s="67">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="V22" s="31"/>
       <c r="W22" s="42">
@@ -4131,7 +4199,7 @@
         <v>117</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -4188,7 +4256,7 @@
         <v>118</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D24" s="12">
         <v>10</v>
@@ -4228,7 +4296,9 @@
       <c r="P24" s="76">
         <v>1</v>
       </c>
-      <c r="Q24" s="76"/>
+      <c r="Q24" s="76">
+        <v>1</v>
+      </c>
       <c r="R24" s="76"/>
       <c r="S24" s="76">
         <v>1</v>
@@ -4236,7 +4306,7 @@
       <c r="T24" s="77"/>
       <c r="U24" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V24" s="31"/>
       <c r="W24" s="14"/>
@@ -4251,7 +4321,7 @@
         <v>119</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D25" s="13">
         <v>8</v>
@@ -4323,10 +4393,10 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D26" s="13">
         <v>3</v>
@@ -4379,7 +4449,7 @@
         <v>120</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D27" s="13">
         <v>3</v>
@@ -4415,12 +4485,15 @@
       <c r="P27" s="75">
         <v>1</v>
       </c>
+      <c r="Q27" s="75">
+        <v>1</v>
+      </c>
       <c r="S27" s="77">
         <v>1</v>
       </c>
       <c r="U27" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V27" s="31"/>
       <c r="W27" s="69">
@@ -4428,15 +4501,15 @@
       </c>
       <c r="X27" s="6">
         <f t="shared" si="2"/>
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="Z27" s="8">
         <f>($Y$17 + $Y$15*X27+$Y$16*Y27)*(1+Y$18+Y$19)</f>
-        <v>28.6</v>
+        <v>31.85</v>
       </c>
       <c r="AA27" s="31"/>
       <c r="AB27" s="31"/>
@@ -4449,7 +4522,7 @@
         <v>121</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D28" s="13">
         <v>3</v>
@@ -4506,15 +4579,15 @@
       </c>
       <c r="X28" s="6">
         <f t="shared" si="2"/>
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="4"/>
-        <v>27.95</v>
+        <v>29.640000000000008</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -4522,7 +4595,7 @@
         <v>122</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D29" s="13">
         <v>5</v>
@@ -4558,15 +4631,15 @@
       </c>
       <c r="X29" s="29">
         <f t="shared" si="2"/>
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="Y29" s="29">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="4"/>
-        <v>17.420000000000002</v>
+        <v>19.89</v>
       </c>
       <c r="AA29" s="31"/>
       <c r="AB29" s="31"/>
@@ -4578,7 +4651,7 @@
         <v>123</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D30" s="13">
         <v>5</v>
@@ -4612,15 +4685,15 @@
       </c>
       <c r="X30" s="6">
         <f t="shared" si="2"/>
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="Y30" s="6">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" si="4"/>
-        <v>16.64</v>
+        <v>18.59</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -4631,7 +4704,7 @@
         <v>124</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D31" s="12">
         <v>3</v>
@@ -4659,15 +4732,13 @@
       <c r="N31" s="76"/>
       <c r="O31" s="76"/>
       <c r="P31" s="76"/>
-      <c r="Q31" s="76">
-        <v>1</v>
-      </c>
+      <c r="Q31" s="76"/>
       <c r="R31" s="76"/>
       <c r="S31" s="76"/>
       <c r="T31" s="77"/>
       <c r="U31" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V31" s="31"/>
       <c r="W31" s="69">
@@ -4675,15 +4746,15 @@
       </c>
       <c r="X31" s="6">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="Y31" s="6">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="4"/>
-        <v>10.530000000000003</v>
+        <v>8.32</v>
       </c>
       <c r="AA31" s="31"/>
       <c r="AB31" s="31"/>
@@ -4695,7 +4766,7 @@
         <v>125</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D32" s="13">
         <v>2</v>
@@ -4756,7 +4827,7 @@
       </c>
       <c r="X32" s="6">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Y32" s="6">
         <f t="shared" si="3"/>
@@ -4764,7 +4835,7 @@
       </c>
       <c r="Z32" s="8">
         <f t="shared" si="4"/>
-        <v>8.1900000000000013</v>
+        <v>8.0600000000000023</v>
       </c>
     </row>
     <row r="33" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4773,7 +4844,7 @@
         <v>186</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="13">
         <v>1</v>
@@ -4827,15 +4898,15 @@
       </c>
       <c r="X33" s="6">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Y33" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z33" s="8">
         <f t="shared" si="4"/>
-        <v>4.8099999999999996</v>
+        <v>6.1099999999999994</v>
       </c>
       <c r="AA33"/>
       <c r="AB33"/>
@@ -4847,7 +4918,7 @@
         <v>187</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D34" s="13">
         <v>3</v>
@@ -4908,15 +4979,15 @@
       </c>
       <c r="X34" s="45">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Y34" s="45">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z34" s="9">
         <f t="shared" si="4"/>
-        <v>4.8099999999999996</v>
+        <v>6.1099999999999994</v>
       </c>
     </row>
     <row r="35" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -4925,7 +4996,7 @@
         <v>126</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D35" s="13">
         <v>3</v>
@@ -4960,12 +5031,12 @@
       <c r="Q35" s="75"/>
       <c r="R35" s="75"/>
       <c r="S35" s="77">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="T35" s="75"/>
       <c r="U35" s="67">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="W35" s="3"/>
       <c r="X35"/>
@@ -4981,7 +5052,7 @@
         <v>97</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D36" s="13">
         <v>2</v>
@@ -5035,7 +5106,7 @@
         <v>98</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D37" s="13">
         <v>4</v>
@@ -5082,7 +5153,7 @@
         <v>95</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D38" s="13">
         <v>3</v>
@@ -5133,7 +5204,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D39" s="13">
         <v>7</v>
@@ -5198,7 +5269,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D40" s="12">
         <v>2</v>
@@ -5262,7 +5333,7 @@
         <v>171</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D41" s="13">
         <v>5</v>
@@ -5322,7 +5393,7 @@
         <v>189</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D42" s="13">
         <v>4</v>
@@ -5369,7 +5440,7 @@
         <v>129</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D43" s="13">
         <v>6</v>
@@ -5419,10 +5490,10 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D44" s="13">
         <v>5</v>
@@ -5461,13 +5532,16 @@
       <c r="O44" s="75">
         <v>1</v>
       </c>
+      <c r="Q44" s="75">
+        <v>1</v>
+      </c>
       <c r="S44" s="77">
         <v>1</v>
       </c>
       <c r="T44" s="78"/>
       <c r="U44" s="81">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V44" s="31"/>
       <c r="Z44" s="6"/>
@@ -5477,10 +5551,10 @@
         <v>79</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D45" s="12">
         <v>7</v>
@@ -5505,7 +5579,7 @@
         <v>26</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L45" s="33">
         <v>1</v>
@@ -5522,29 +5596,25 @@
       <c r="P45" s="76">
         <v>1</v>
       </c>
-      <c r="Q45" s="76">
-        <v>1</v>
-      </c>
-      <c r="R45" s="76">
-        <v>1</v>
-      </c>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="76"/>
       <c r="S45" s="76">
         <v>1</v>
       </c>
       <c r="T45" s="77"/>
       <c r="U45" s="67">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V45" s="31"/>
     </row>
     <row r="46" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="28"/>
       <c r="B46" s="29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D46" s="13">
         <v>4</v>
@@ -5561,20 +5631,24 @@
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
       <c r="K46" s="21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="L46" s="77"/>
       <c r="M46" s="77"/>
       <c r="N46" s="77"/>
       <c r="O46" s="77"/>
       <c r="P46" s="77"/>
-      <c r="Q46" s="77"/>
-      <c r="R46" s="77"/>
+      <c r="Q46" s="77">
+        <v>1</v>
+      </c>
+      <c r="R46" s="77">
+        <v>1</v>
+      </c>
       <c r="S46" s="77"/>
       <c r="T46" s="77"/>
       <c r="U46" s="67">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W46" s="3"/>
     </row>
@@ -5583,7 +5657,7 @@
         <v>93</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D47" s="13">
         <v>6</v>
@@ -5608,7 +5682,7 @@
         <v>27</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L47" s="32">
         <v>1</v>
@@ -5625,18 +5699,12 @@
       <c r="P47" s="75">
         <v>1</v>
       </c>
-      <c r="Q47" s="75">
-        <v>1</v>
-      </c>
-      <c r="R47" s="75">
-        <v>1</v>
-      </c>
       <c r="S47" s="77">
         <v>0.9</v>
       </c>
       <c r="U47" s="67">
         <f t="shared" si="1"/>
-        <v>2.9</v>
+        <v>0.9</v>
       </c>
       <c r="V47" s="31"/>
       <c r="Z47" s="6"/>
@@ -5648,10 +5716,10 @@
     <row r="48" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="22" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D48" s="13">
         <v>8</v>
@@ -5668,20 +5736,24 @@
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="L48" s="75"/>
       <c r="M48" s="75"/>
       <c r="N48" s="75"/>
       <c r="O48" s="75"/>
       <c r="P48" s="75"/>
-      <c r="Q48" s="75"/>
-      <c r="R48" s="75"/>
+      <c r="Q48" s="75">
+        <v>1</v>
+      </c>
+      <c r="R48" s="75">
+        <v>1</v>
+      </c>
       <c r="S48" s="77"/>
       <c r="T48" s="75"/>
       <c r="U48" s="67">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W48" s="3"/>
       <c r="Z48" s="6"/>
@@ -5696,7 +5768,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D49" s="13">
         <v>2</v>
@@ -5741,12 +5813,12 @@
         <v>1</v>
       </c>
       <c r="S49" s="77">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="T49" s="75"/>
       <c r="U49" s="67">
         <f t="shared" si="1"/>
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V49" s="31"/>
       <c r="W49" s="14"/>
@@ -5759,10 +5831,10 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B50" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D50" s="13">
         <v>4</v>
@@ -5787,18 +5859,23 @@
         <v>28</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="L50" s="32"/>
       <c r="M50" s="32"/>
       <c r="O50" s="75">
         <v>0.75</v>
       </c>
-      <c r="S50" s="77"/>
+      <c r="P50" s="75">
+        <v>1</v>
+      </c>
+      <c r="S50" s="77">
+        <v>1</v>
+      </c>
       <c r="T50" s="78"/>
       <c r="U50" s="81">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="31"/>
       <c r="Y50" s="6"/>
@@ -5808,10 +5885,10 @@
         <v>80</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D51" s="12">
         <v>2</v>
@@ -5863,7 +5940,7 @@
         <v>131</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D52" s="13">
         <v>3</v>
@@ -5925,7 +6002,7 @@
         <v>132</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D53" s="12">
         <v>2</v>
@@ -5979,7 +6056,7 @@
         <v>133</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D54" s="13">
         <v>3</v>
@@ -6044,7 +6121,7 @@
         <v>134</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D55" s="13">
         <v>3</v>
@@ -6073,7 +6150,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="75">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R55" s="75">
         <v>1</v>
@@ -6083,7 +6160,7 @@
       </c>
       <c r="U55" s="67">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V55" s="31"/>
     </row>
@@ -6092,7 +6169,7 @@
         <v>135</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D56" s="13">
         <v>3</v>
@@ -6133,7 +6210,7 @@
         <v>136</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" s="13">
         <v>2</v>
@@ -6177,11 +6254,11 @@
         <v>1</v>
       </c>
       <c r="S57" s="77">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="U57" s="67">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="V57" s="31"/>
       <c r="AA57" s="31"/>
@@ -6191,7 +6268,7 @@
         <v>137</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D58" s="13">
         <v>5</v>
@@ -6249,7 +6326,7 @@
         <v>138</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D59" s="13">
         <v>5</v>
@@ -6290,11 +6367,11 @@
         <v>1</v>
       </c>
       <c r="S59" s="77">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="U59" s="67">
         <f t="shared" si="1"/>
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V59" s="31"/>
       <c r="Y59" s="6"/>
@@ -6305,7 +6382,7 @@
         <v>139</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D60" s="13">
         <v>1</v>
@@ -6362,7 +6439,7 @@
         <v>96</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D61" s="13">
         <v>3</v>
@@ -6403,7 +6480,7 @@
         <v>140</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D62" s="13">
         <v>5</v>
@@ -6445,7 +6522,7 @@
         <v>141</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D63" s="13">
         <v>9</v>
@@ -6481,7 +6558,7 @@
         <v>142</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D64" s="13">
         <v>7</v>
@@ -6521,7 +6598,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D65" s="13">
         <v>5</v>
@@ -6546,6 +6623,9 @@
       <c r="O65" s="75">
         <v>0.5</v>
       </c>
+      <c r="P65" s="75">
+        <v>1</v>
+      </c>
       <c r="S65" s="77">
         <v>1</v>
       </c>
@@ -6566,7 +6646,7 @@
         <v>144</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D66" s="12">
         <v>3</v>
@@ -6621,7 +6701,7 @@
         <v>145</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D67" s="13">
         <v>7</v>
@@ -6670,7 +6750,7 @@
         <v>146</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D68" s="13">
         <v>7</v>
@@ -6701,7 +6781,7 @@
         <v>147</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D69" s="26">
         <v>10</v>
@@ -6747,7 +6827,7 @@
         <v>148</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D70" s="13">
         <v>4</v>
@@ -6762,9 +6842,7 @@
       <c r="G70" s="13">
         <v>48</v>
       </c>
-      <c r="K70" s="21" t="s">
-        <v>195</v>
-      </c>
+      <c r="K70" s="21"/>
       <c r="L70" s="32"/>
       <c r="M70" s="31"/>
       <c r="S70" s="77"/>
@@ -6782,7 +6860,7 @@
         <v>149</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D71" s="13">
         <v>3</v>
@@ -6826,10 +6904,10 @@
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B72" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D72" s="13">
         <v>4</v>
@@ -6842,7 +6920,7 @@
         <v>4</v>
       </c>
       <c r="K72" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L72" s="75"/>
       <c r="M72" s="75"/>
@@ -6899,12 +6977,12 @@
       <c r="Q73" s="76"/>
       <c r="R73" s="76"/>
       <c r="S73" s="76">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="T73" s="77"/>
       <c r="U73" s="67">
         <f t="shared" si="7"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="W73" s="3"/>
       <c r="X73"/>
@@ -6932,7 +7010,7 @@
         <v>2</v>
       </c>
       <c r="K74" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L74" s="34"/>
       <c r="M74" s="34">
@@ -6949,18 +7027,20 @@
       </c>
       <c r="Q74" s="77"/>
       <c r="R74" s="77"/>
-      <c r="S74" s="77"/>
+      <c r="S74" s="77">
+        <v>1</v>
+      </c>
       <c r="T74" s="77"/>
       <c r="U74" s="67">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V74" s="31"/>
     </row>
     <row r="75" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="28"/>
       <c r="B75" s="29" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="13">
@@ -6978,7 +7058,7 @@
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="21" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="L75" s="77"/>
       <c r="M75" s="77"/>
@@ -6986,7 +7066,9 @@
       <c r="O75" s="77"/>
       <c r="P75" s="77"/>
       <c r="Q75" s="77"/>
-      <c r="R75" s="77"/>
+      <c r="R75" s="77">
+        <v>1</v>
+      </c>
       <c r="S75" s="77">
         <v>1</v>
       </c>
@@ -6995,7 +7077,7 @@
       </c>
       <c r="U75" s="67">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W75" s="3"/>
     </row>
@@ -7178,7 +7260,7 @@
     <row r="81" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10"/>
       <c r="B81" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C81" s="23"/>
       <c r="D81" s="26">
@@ -7196,7 +7278,7 @@
       <c r="I81" s="26"/>
       <c r="J81" s="26"/>
       <c r="K81" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L81" s="35"/>
       <c r="M81" s="35">
@@ -7245,15 +7327,15 @@
       </c>
       <c r="Q83" s="61">
         <f t="array" ref="Q83">SUM($F2:$F81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="R83" s="61">
         <f t="array" ref="R83">SUM($F2:$F81*(R2:R81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="S83" s="61">
         <f t="array" ref="S83">SUM($F2:$F81*(S2:S81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="T83" s="63"/>
       <c r="X83" s="31"/>
@@ -7275,15 +7357,15 @@
       </c>
       <c r="Q84" s="63">
         <f t="array" ref="Q84">SUM($F2:$F81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="R84" s="63">
         <f t="array" ref="R84">SUM($F2:$F81*R2:R81*($U2:$U81&gt;=$W$12))</f>
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="S84" s="63">
         <f t="array" ref="S84">SUM($F2:$F81*S2:S81*($U2:$U81&gt;=$W$12))</f>
-        <v>121.80000000000001</v>
+        <v>177.39999999999998</v>
       </c>
       <c r="T84" s="63"/>
       <c r="AA84" s="6"/>
@@ -7302,15 +7384,15 @@
       </c>
       <c r="Q85" s="63">
         <f t="array" ref="Q85">SUM($F$2:$F$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="R85" s="63">
         <f t="array" ref="R85">SUM($F$2:$F$81*(R$2:R$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="S85" s="63">
         <f t="array" ref="S85">SUM($F$2:$F$81*(S$2:S$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="T85" s="63"/>
     </row>
@@ -7325,15 +7407,15 @@
       </c>
       <c r="Q86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="R86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="S86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="T86" s="63"/>
     </row>
@@ -7348,15 +7430,15 @@
       </c>
       <c r="Q87" s="64">
         <f t="shared" ref="Q87:S87" si="8">Q84/Q86</f>
-        <v>0.41221374045801529</v>
+        <v>0.60606060606060608</v>
       </c>
       <c r="R87" s="64">
         <f t="shared" si="8"/>
-        <v>0.38931297709923662</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="S87" s="64">
         <f t="shared" si="8"/>
-        <v>0.46488549618320613</v>
+        <v>0.67196969696969688</v>
       </c>
       <c r="T87" s="64"/>
     </row>
@@ -7372,15 +7454,15 @@
       </c>
       <c r="Q88" s="66">
         <f t="array" ref="Q88">SUM($F2:$F81*Q2:Q81*($U2:$U81&lt;$W$12))</f>
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="R88" s="66">
         <f t="array" ref="R88">SUM($F2:$F81*R2:R81*($U2:$U81&lt;$W$12))</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="S88" s="66">
         <f t="array" ref="S88">SUM($F2:$F81*S2:S81*($U2:$U81&lt;$W$12))</f>
-        <v>59.2</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="T88" s="63"/>
       <c r="Z88" s="31"/>
@@ -7421,6 +7503,34 @@
       <c r="AB91"/>
       <c r="AC91"/>
       <c r="AD91"/>
+    </row>
+    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="N92" s="75" t="s">
+        <v>233</v>
+      </c>
+      <c r="P92" s="75" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q92" s="75" t="s">
+        <v>235</v>
+      </c>
+      <c r="R92" s="75" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="P93" s="75">
+        <f>SUMPRODUCT(R4:R81,Q4:Q81,$F4:$F81)</f>
+        <v>62</v>
+      </c>
+      <c r="Q93" s="75">
+        <f t="shared" ref="Q93:R93" si="9">SUMPRODUCT(S4:S81,R4:R81,$F4:$F81)</f>
+        <v>76.400000000000006</v>
+      </c>
+      <c r="R93" s="75">
+        <f>SUMPRODUCT(S4:S81,Q4:Q81,$F4:$F81)</f>
+        <v>83.2</v>
+      </c>
     </row>
     <row r="97" spans="27:30" x14ac:dyDescent="0.3">
       <c r="AA97" s="6"/>

</xml_diff>

<commit_message>
Finalized spring 2020 spreadsheet
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2020spring.xlsx
@@ -15,7 +15,7 @@
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -1581,9 +1581,6 @@
     <t>Using 32-bit applications in Windows</t>
   </si>
   <si>
-    <t>Needed for kinetic theory labs</t>
-  </si>
-  <si>
     <t>Kirchoff's Rules</t>
   </si>
   <si>
@@ -1701,6 +1698,9 @@
   </si>
   <si>
     <t>gpg&amp;mt</t>
+  </si>
+  <si>
+    <t>Needed for kinetic theory labs?</t>
   </si>
 </sst>
 </file>
@@ -2573,49 +2573,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -2948,9 +2906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2959,8 +2917,8 @@
     <col min="2" max="2" width="53.77734375" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" style="22" customWidth="1"/>
     <col min="4" max="4" width="8.109375" style="13" customWidth="1"/>
-    <col min="5" max="6" width="5.77734375" style="13" customWidth="1"/>
-    <col min="7" max="10" width="5.77734375" style="13" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="5.77734375" style="13" customWidth="1"/>
+    <col min="6" max="10" width="5.77734375" style="13" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="30.109375" style="19" customWidth="1"/>
     <col min="12" max="13" width="8.77734375" style="2" customWidth="1"/>
     <col min="14" max="20" width="8.77734375" style="75" customWidth="1"/>
@@ -2979,7 +2937,7 @@
         <v>107</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D1" s="48" t="s">
         <v>85</v>
@@ -2988,7 +2946,7 @@
         <v>86</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G1" s="48" t="s">
         <v>176</v>
@@ -3012,28 +2970,28 @@
         <v>195</v>
       </c>
       <c r="N1" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="O1" s="47" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="47" t="s">
-        <v>213</v>
-      </c>
       <c r="P1" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q1" s="47" t="s">
+        <v>221</v>
+      </c>
+      <c r="R1" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="S1" s="47" t="s">
         <v>223</v>
       </c>
-      <c r="S1" s="47" t="s">
-        <v>224</v>
-      </c>
       <c r="T1" s="47" t="s">
+        <v>219</v>
+      </c>
+      <c r="U1" s="50" t="s">
         <v>220</v>
-      </c>
-      <c r="U1" s="50" t="s">
-        <v>221</v>
       </c>
       <c r="V1" s="30"/>
       <c r="W1" s="31"/>
@@ -3159,7 +3117,7 @@
         <v>110</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="13">
         <v>5</v>
@@ -3228,7 +3186,7 @@
         <v>156</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="13">
         <v>2</v>
@@ -3294,7 +3252,7 @@
         <v>157</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="13">
         <v>2</v>
@@ -3350,7 +3308,7 @@
         <v>180</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" s="26">
         <v>1</v>
@@ -3397,7 +3355,7 @@
         <v>172</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D8" s="13">
         <v>4</v>
@@ -3458,7 +3416,7 @@
         <v>111</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="13">
         <v>2</v>
@@ -3519,7 +3477,7 @@
         <v>112</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" s="13">
         <v>5</v>
@@ -3568,7 +3526,7 @@
         <v>113</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11" s="13">
         <v>2</v>
@@ -3628,10 +3586,10 @@
     </row>
     <row r="12" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="13">
         <v>4</v>
@@ -3644,7 +3602,7 @@
         <v>4</v>
       </c>
       <c r="K12" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L12" s="75"/>
       <c r="M12" s="75"/>
@@ -3678,10 +3636,10 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" s="13">
         <v>3</v>
@@ -3694,7 +3652,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L13" s="75"/>
       <c r="M13" s="75"/>
@@ -3726,10 +3684,10 @@
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D14" s="13">
         <v>3</v>
@@ -3742,7 +3700,7 @@
         <v>4</v>
       </c>
       <c r="K14" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L14" s="75"/>
       <c r="M14" s="75"/>
@@ -3764,10 +3722,10 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="13">
         <v>3</v>
@@ -3780,7 +3738,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L15" s="75"/>
       <c r="M15" s="75"/>
@@ -3808,7 +3766,7 @@
         <v>182</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D16" s="13">
         <v>9</v>
@@ -3841,12 +3799,15 @@
       <c r="Q16" s="75">
         <v>1</v>
       </c>
+      <c r="R16" s="75">
+        <v>1</v>
+      </c>
       <c r="S16" s="77">
         <v>1</v>
       </c>
       <c r="U16" s="67">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V16" s="31"/>
       <c r="W16" s="17" t="s">
@@ -3867,7 +3828,7 @@
         <v>185</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D17" s="13">
         <v>3</v>
@@ -3939,7 +3900,7 @@
         <v>183</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D18" s="13">
         <v>5</v>
@@ -3967,14 +3928,14 @@
         <v>0.5</v>
       </c>
       <c r="R18" s="75">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S18" s="77">
         <v>1</v>
       </c>
       <c r="U18" s="67">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V18" s="31"/>
       <c r="W18" s="17" t="s">
@@ -3995,7 +3956,7 @@
         <v>184</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D19" s="13">
         <v>4</v>
@@ -4029,14 +3990,14 @@
         <v>1</v>
       </c>
       <c r="R19" s="75">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="S19" s="77">
         <v>1</v>
       </c>
       <c r="U19" s="67">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2.1</v>
       </c>
       <c r="V19" s="31"/>
       <c r="W19" s="18" t="s">
@@ -4057,7 +4018,7 @@
         <v>114</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" s="13">
         <v>5</v>
@@ -4094,14 +4055,14 @@
         <v>1</v>
       </c>
       <c r="R20" s="75">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="S20" s="77">
         <v>1</v>
       </c>
       <c r="U20" s="67">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="V20" s="31"/>
       <c r="Z20" s="31"/>
@@ -4115,7 +4076,7 @@
         <v>115</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="13">
         <v>3</v>
@@ -4140,7 +4101,7 @@
       </c>
       <c r="V21" s="31"/>
       <c r="W21" s="40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X21" s="41"/>
       <c r="Y21" s="31"/>
@@ -4155,7 +4116,7 @@
         <v>116</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D22" s="13">
         <v>4</v>
@@ -4199,7 +4160,7 @@
         <v>117</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
@@ -4256,7 +4217,7 @@
         <v>118</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D24" s="12">
         <v>10</v>
@@ -4299,14 +4260,16 @@
       <c r="Q24" s="76">
         <v>1</v>
       </c>
-      <c r="R24" s="76"/>
+      <c r="R24" s="76">
+        <v>1</v>
+      </c>
       <c r="S24" s="76">
         <v>1</v>
       </c>
       <c r="T24" s="77"/>
       <c r="U24" s="67">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V24" s="31"/>
       <c r="W24" s="14"/>
@@ -4321,7 +4284,7 @@
         <v>119</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="13">
         <v>8</v>
@@ -4393,10 +4356,10 @@
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D26" s="13">
         <v>3</v>
@@ -4449,7 +4412,7 @@
         <v>120</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" s="13">
         <v>3</v>
@@ -4501,7 +4464,7 @@
       </c>
       <c r="X27" s="6">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Y27" s="6">
         <f t="shared" si="3"/>
@@ -4509,7 +4472,7 @@
       </c>
       <c r="Z27" s="8">
         <f>($Y$17 + $Y$15*X27+$Y$16*Y27)*(1+Y$18+Y$19)</f>
-        <v>31.85</v>
+        <v>31.72</v>
       </c>
       <c r="AA27" s="31"/>
       <c r="AB27" s="31"/>
@@ -4522,7 +4485,7 @@
         <v>121</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="13">
         <v>3</v>
@@ -4579,7 +4542,7 @@
       </c>
       <c r="X28" s="6">
         <f t="shared" si="2"/>
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="Y28" s="6">
         <f t="shared" si="3"/>
@@ -4587,7 +4550,7 @@
       </c>
       <c r="Z28" s="8">
         <f t="shared" si="4"/>
-        <v>29.640000000000008</v>
+        <v>29.510000000000005</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
@@ -4595,7 +4558,7 @@
         <v>122</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D29" s="13">
         <v>5</v>
@@ -4631,15 +4594,15 @@
       </c>
       <c r="X29" s="29">
         <f t="shared" si="2"/>
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="Y29" s="29">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z29" s="8">
         <f t="shared" si="4"/>
-        <v>19.89</v>
+        <v>20.540000000000003</v>
       </c>
       <c r="AA29" s="31"/>
       <c r="AB29" s="31"/>
@@ -4651,7 +4614,7 @@
         <v>123</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="13">
         <v>5</v>
@@ -4685,15 +4648,15 @@
       </c>
       <c r="X30" s="6">
         <f t="shared" si="2"/>
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="Y30" s="6">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z30" s="8">
         <f t="shared" si="4"/>
-        <v>18.59</v>
+        <v>20.28</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
@@ -4704,7 +4667,7 @@
         <v>124</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" s="12">
         <v>3</v>
@@ -4746,15 +4709,15 @@
       </c>
       <c r="X31" s="6">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="Y31" s="6">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z31" s="8">
         <f t="shared" si="4"/>
-        <v>8.32</v>
+        <v>11.57</v>
       </c>
       <c r="AA31" s="31"/>
       <c r="AB31" s="31"/>
@@ -4766,7 +4729,7 @@
         <v>125</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D32" s="13">
         <v>2</v>
@@ -4827,15 +4790,15 @@
       </c>
       <c r="X32" s="6">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="Y32" s="6">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Z32" s="8">
         <f t="shared" si="4"/>
-        <v>8.0600000000000023</v>
+        <v>11.309999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4844,7 +4807,7 @@
         <v>186</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D33" s="13">
         <v>1</v>
@@ -4883,14 +4846,16 @@
       <c r="Q33" s="75">
         <v>1</v>
       </c>
-      <c r="R33" s="75"/>
+      <c r="R33" s="75">
+        <v>1</v>
+      </c>
       <c r="S33" s="77">
         <v>0</v>
       </c>
       <c r="T33" s="75"/>
       <c r="U33" s="67">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V33" s="31"/>
       <c r="W33" s="69">
@@ -4918,7 +4883,7 @@
         <v>187</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D34" s="13">
         <v>3</v>
@@ -4996,7 +4961,7 @@
         <v>126</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D35" s="13">
         <v>3</v>
@@ -5052,7 +5017,7 @@
         <v>97</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D36" s="13">
         <v>2</v>
@@ -5106,7 +5071,7 @@
         <v>98</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D37" s="13">
         <v>4</v>
@@ -5153,7 +5118,7 @@
         <v>95</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D38" s="13">
         <v>3</v>
@@ -5204,7 +5169,7 @@
         <v>127</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D39" s="13">
         <v>7</v>
@@ -5269,7 +5234,7 @@
         <v>128</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D40" s="12">
         <v>2</v>
@@ -5333,7 +5298,7 @@
         <v>171</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="13">
         <v>5</v>
@@ -5393,7 +5358,7 @@
         <v>189</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D42" s="13">
         <v>4</v>
@@ -5440,7 +5405,7 @@
         <v>129</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D43" s="13">
         <v>6</v>
@@ -5490,10 +5455,10 @@
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D44" s="13">
         <v>5</v>
@@ -5551,10 +5516,10 @@
         <v>79</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D45" s="12">
         <v>7</v>
@@ -5579,7 +5544,7 @@
         <v>26</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L45" s="33">
         <v>1</v>
@@ -5611,10 +5576,10 @@
     <row r="46" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="28"/>
       <c r="B46" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D46" s="13">
         <v>4</v>
@@ -5631,7 +5596,7 @@
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
       <c r="K46" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L46" s="77"/>
       <c r="M46" s="77"/>
@@ -5657,7 +5622,7 @@
         <v>93</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D47" s="13">
         <v>6</v>
@@ -5682,7 +5647,7 @@
         <v>27</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L47" s="32">
         <v>1</v>
@@ -5716,10 +5681,10 @@
     <row r="48" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
       <c r="B48" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="13">
         <v>8</v>
@@ -5736,7 +5701,7 @@
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
       <c r="K48" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L48" s="75"/>
       <c r="M48" s="75"/>
@@ -5768,7 +5733,7 @@
         <v>130</v>
       </c>
       <c r="C49" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D49" s="13">
         <v>2</v>
@@ -5831,10 +5796,10 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B50" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D50" s="13">
         <v>4</v>
@@ -5859,7 +5824,7 @@
         <v>28</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L50" s="32"/>
       <c r="M50" s="32"/>
@@ -5885,10 +5850,10 @@
         <v>80</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="12">
         <v>2</v>
@@ -5940,7 +5905,7 @@
         <v>131</v>
       </c>
       <c r="C52" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D52" s="13">
         <v>3</v>
@@ -6002,7 +5967,7 @@
         <v>132</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D53" s="12">
         <v>2</v>
@@ -6056,7 +6021,7 @@
         <v>133</v>
       </c>
       <c r="C54" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D54" s="13">
         <v>3</v>
@@ -6121,7 +6086,7 @@
         <v>134</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D55" s="13">
         <v>3</v>
@@ -6169,7 +6134,7 @@
         <v>135</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D56" s="13">
         <v>3</v>
@@ -6210,7 +6175,7 @@
         <v>136</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D57" s="13">
         <v>2</v>
@@ -6268,7 +6233,7 @@
         <v>137</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D58" s="13">
         <v>5</v>
@@ -6326,7 +6291,7 @@
         <v>138</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D59" s="13">
         <v>5</v>
@@ -6382,7 +6347,7 @@
         <v>139</v>
       </c>
       <c r="C60" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D60" s="13">
         <v>1</v>
@@ -6439,7 +6404,7 @@
         <v>96</v>
       </c>
       <c r="C61" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D61" s="13">
         <v>3</v>
@@ -6480,7 +6445,7 @@
         <v>140</v>
       </c>
       <c r="C62" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D62" s="13">
         <v>5</v>
@@ -6507,6 +6472,9 @@
       <c r="O62" s="75">
         <v>0.5</v>
       </c>
+      <c r="P62" s="75">
+        <v>1</v>
+      </c>
       <c r="S62" s="77">
         <v>1</v>
       </c>
@@ -6522,7 +6490,7 @@
         <v>141</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D63" s="13">
         <v>9</v>
@@ -6558,7 +6526,7 @@
         <v>142</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D64" s="13">
         <v>7</v>
@@ -6598,7 +6566,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D65" s="13">
         <v>5</v>
@@ -6646,7 +6614,7 @@
         <v>144</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D66" s="12">
         <v>3</v>
@@ -6683,14 +6651,16 @@
       <c r="Q66" s="76">
         <v>1</v>
       </c>
-      <c r="R66" s="76"/>
+      <c r="R66" s="76">
+        <v>1</v>
+      </c>
       <c r="S66" s="76">
         <v>0.5</v>
       </c>
       <c r="T66" s="77"/>
       <c r="U66" s="67">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="V66" s="31"/>
       <c r="AA66" s="31"/>
@@ -6701,7 +6671,7 @@
         <v>145</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D67" s="13">
         <v>7</v>
@@ -6750,7 +6720,7 @@
         <v>146</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D68" s="13">
         <v>7</v>
@@ -6781,7 +6751,7 @@
         <v>147</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D69" s="26">
         <v>10</v>
@@ -6827,7 +6797,7 @@
         <v>148</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D70" s="13">
         <v>4</v>
@@ -6860,7 +6830,7 @@
         <v>149</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D71" s="13">
         <v>3</v>
@@ -6904,10 +6874,10 @@
     </row>
     <row r="72" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B72" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D72" s="13">
         <v>4</v>
@@ -6920,7 +6890,7 @@
         <v>4</v>
       </c>
       <c r="K72" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L72" s="75"/>
       <c r="M72" s="75"/>
@@ -7010,7 +6980,7 @@
         <v>2</v>
       </c>
       <c r="K74" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L74" s="34"/>
       <c r="M74" s="34">
@@ -7025,22 +6995,26 @@
       <c r="P74" s="77">
         <v>1</v>
       </c>
-      <c r="Q74" s="77"/>
-      <c r="R74" s="77"/>
+      <c r="Q74" s="77">
+        <v>1</v>
+      </c>
+      <c r="R74" s="77">
+        <v>1</v>
+      </c>
       <c r="S74" s="77">
         <v>1</v>
       </c>
       <c r="T74" s="77"/>
       <c r="U74" s="67">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V74" s="31"/>
     </row>
     <row r="75" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="28"/>
       <c r="B75" s="29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C75" s="29"/>
       <c r="D75" s="13">
@@ -7058,14 +7032,16 @@
       <c r="I75" s="13"/>
       <c r="J75" s="13"/>
       <c r="K75" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L75" s="77"/>
       <c r="M75" s="77"/>
       <c r="N75" s="77"/>
       <c r="O75" s="77"/>
       <c r="P75" s="77"/>
-      <c r="Q75" s="77"/>
+      <c r="Q75" s="77">
+        <v>1</v>
+      </c>
       <c r="R75" s="77">
         <v>1</v>
       </c>
@@ -7077,7 +7053,7 @@
       </c>
       <c r="U75" s="67">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W75" s="3"/>
     </row>
@@ -7108,6 +7084,9 @@
       <c r="O76" s="75">
         <v>1</v>
       </c>
+      <c r="Q76" s="75">
+        <v>1</v>
+      </c>
       <c r="R76" s="75">
         <v>1</v>
       </c>
@@ -7116,7 +7095,7 @@
       </c>
       <c r="U76" s="67">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V76" s="31"/>
       <c r="X76" s="31"/>
@@ -7161,7 +7140,9 @@
       <c r="P77" s="75">
         <v>1</v>
       </c>
-      <c r="Q77" s="75"/>
+      <c r="Q77" s="75">
+        <v>1</v>
+      </c>
       <c r="R77" s="75"/>
       <c r="S77" s="77">
         <v>1</v>
@@ -7169,7 +7150,7 @@
       <c r="T77" s="75"/>
       <c r="U77" s="67">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V77" s="14"/>
       <c r="W77" s="3"/>
@@ -7278,7 +7259,7 @@
       <c r="I81" s="26"/>
       <c r="J81" s="26"/>
       <c r="K81" s="27" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="L81" s="35"/>
       <c r="M81" s="35">
@@ -7291,17 +7272,13 @@
       <c r="P81" s="78">
         <v>1</v>
       </c>
-      <c r="Q81" s="78">
-        <v>1</v>
-      </c>
+      <c r="Q81" s="78"/>
       <c r="R81" s="78"/>
-      <c r="S81" s="78">
-        <v>1</v>
-      </c>
+      <c r="S81" s="78"/>
       <c r="T81" s="78"/>
       <c r="U81" s="81">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V81" s="14"/>
       <c r="W81" s="3"/>
@@ -7327,15 +7304,15 @@
       </c>
       <c r="Q83" s="61">
         <f t="array" ref="Q83">SUM($F2:$F81*(Q2:Q81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="R83" s="61">
         <f t="array" ref="R83">SUM($F2:$F81*(R2:R81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>112</v>
+        <v>152</v>
       </c>
       <c r="S83" s="61">
         <f t="array" ref="S83">SUM($F2:$F81*(S2:S81&gt;=0.9)*($U2:$U81&gt;=$W$12))</f>
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="T83" s="63"/>
       <c r="X83" s="31"/>
@@ -7357,15 +7334,15 @@
       </c>
       <c r="Q84" s="63">
         <f t="array" ref="Q84">SUM($F2:$F81*Q2:Q81*($U2:$U81&gt;=$W$12))</f>
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="R84" s="63">
         <f t="array" ref="R84">SUM($F2:$F81*R2:R81*($U2:$U81&gt;=$W$12))</f>
-        <v>120</v>
+        <v>152.4</v>
       </c>
       <c r="S84" s="63">
         <f t="array" ref="S84">SUM($F2:$F81*S2:S81*($U2:$U81&gt;=$W$12))</f>
-        <v>177.39999999999998</v>
+        <v>175.39999999999998</v>
       </c>
       <c r="T84" s="63"/>
       <c r="AA84" s="6"/>
@@ -7384,15 +7361,15 @@
       </c>
       <c r="Q85" s="63">
         <f t="array" ref="Q85">SUM($F$2:$F$81*(Q$2:Q$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="R85" s="63">
         <f t="array" ref="R85">SUM($F$2:$F$81*(R$2:R$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="S85" s="63">
         <f t="array" ref="S85">SUM($F$2:$F$81*(S$2:S$81&gt;=0.1)*($U$2:$U$81&gt;=$W$12))</f>
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T85" s="63"/>
     </row>
@@ -7407,15 +7384,15 @@
       </c>
       <c r="Q86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="S86" s="63">
         <f>LOOKUP($W$12,$W26:$W34,$X26:$X34)</f>
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T86" s="63"/>
     </row>
@@ -7430,15 +7407,15 @@
       </c>
       <c r="Q87" s="64">
         <f t="shared" ref="Q87:S87" si="8">Q84/Q86</f>
-        <v>0.60606060606060608</v>
+        <v>0.64122137404580148</v>
       </c>
       <c r="R87" s="64">
         <f t="shared" si="8"/>
-        <v>0.45454545454545453</v>
+        <v>0.58167938931297714</v>
       </c>
       <c r="S87" s="64">
         <f t="shared" si="8"/>
-        <v>0.67196969696969688</v>
+        <v>0.66946564885496174</v>
       </c>
       <c r="T87" s="64"/>
     </row>
@@ -7506,30 +7483,30 @@
     </row>
     <row r="92" spans="1:30" x14ac:dyDescent="0.3">
       <c r="N92" s="75" t="s">
+        <v>232</v>
+      </c>
+      <c r="P92" s="75" t="s">
         <v>233</v>
       </c>
-      <c r="P92" s="75" t="s">
+      <c r="Q92" s="75" t="s">
         <v>234</v>
       </c>
-      <c r="Q92" s="75" t="s">
+      <c r="R92" s="75" t="s">
         <v>235</v>
-      </c>
-      <c r="R92" s="75" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="93" spans="1:30" x14ac:dyDescent="0.3">
       <c r="P93" s="75">
         <f>SUMPRODUCT(R4:R81,Q4:Q81,$F4:$F81)</f>
-        <v>62</v>
+        <v>94.4</v>
       </c>
       <c r="Q93" s="75">
-        <f t="shared" ref="Q93:R93" si="9">SUMPRODUCT(S4:S81,R4:R81,$F4:$F81)</f>
-        <v>76.400000000000006</v>
+        <f t="shared" ref="Q93" si="9">SUMPRODUCT(S4:S81,R4:R81,$F4:$F81)</f>
+        <v>104.80000000000001</v>
       </c>
       <c r="R93" s="75">
         <f>SUMPRODUCT(S4:S81,Q4:Q81,$F4:$F81)</f>
-        <v>83.2</v>
+        <v>91.2</v>
       </c>
     </row>
     <row r="97" spans="27:30" x14ac:dyDescent="0.3">

</xml_diff>